<commit_message>
CuAu fcc-cube run (up to 4.5ish nm)
</commit_message>
<xml_diff>
--- a/data/bimetallic_results/fcc-cube/fcc-cube_CuAu_data_sub5.xlsx
+++ b/data/bimetallic_results/fcc-cube/fcc-cube_CuAu_data_sub5.xlsx
@@ -386,7 +386,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E79"/>
+  <dimension ref="A1:E189"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -709,10 +709,10 @@
         <v>0.04761904761904762</v>
       </c>
       <c r="D19">
-        <v>-2.789574110896522</v>
+        <v>-2.789574110896523</v>
       </c>
       <c r="E19">
-        <v>-0.04987644809126612</v>
+        <v>-0.04987644809126657</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -760,10 +760,10 @@
         <v>0.09523809523809523</v>
       </c>
       <c r="D22">
-        <v>-2.847575278058019</v>
+        <v>-2.850098872509298</v>
       </c>
       <c r="E22">
-        <v>-0.09596750450561364</v>
+        <v>-0.09849109895689256</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -777,10 +777,10 @@
         <v>0.1111111111111111</v>
       </c>
       <c r="D23">
-        <v>-2.868170797670824</v>
+        <v>-2.863006937906288</v>
       </c>
       <c r="E23">
-        <v>-0.1125929872027021</v>
+        <v>-0.107429127438166</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -794,10 +794,10 @@
         <v>0.126984126984127</v>
       </c>
       <c r="D24">
-        <v>-2.89002811450927</v>
+        <v>-2.882340660293454</v>
       </c>
       <c r="E24">
-        <v>-0.130480267125431</v>
+        <v>-0.1227928129096152</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -811,10 +811,10 @@
         <v>0.1428571428571428</v>
       </c>
       <c r="D25">
-        <v>-2.904197977131899</v>
+        <v>-2.908100039670796</v>
       </c>
       <c r="E25">
-        <v>-0.1406800928323442</v>
+        <v>-0.1445821553712405</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -828,10 +828,10 @@
         <v>0.1587301587301587</v>
       </c>
       <c r="D26">
-        <v>-2.924793496744704</v>
+        <v>-2.921349138483738</v>
       </c>
       <c r="E26">
-        <v>-0.1573055755294321</v>
+        <v>-0.1538612172684659</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -845,10 +845,10 @@
         <v>0.1746031746031746</v>
       </c>
       <c r="D27">
-        <v>-2.946767484445127</v>
+        <v>-2.920945725379538</v>
       </c>
       <c r="E27">
-        <v>-0.1753095263141389</v>
+        <v>-0.1494877672485502</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -862,10 +862,10 @@
         <v>0.1904761904761905</v>
       </c>
       <c r="D28">
-        <v>-2.956114520719172</v>
+        <v>-2.954852723493532</v>
       </c>
       <c r="E28">
-        <v>-0.1806865256724675</v>
+        <v>-0.1794247284468273</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -879,10 +879,10 @@
         <v>0.2063492063492063</v>
       </c>
       <c r="D29">
-        <v>-2.956883900784172</v>
+        <v>-2.95176037625595</v>
       </c>
       <c r="E29">
-        <v>-0.1774858688217504</v>
+        <v>-0.172362344293528</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -896,10 +896,10 @@
         <v>0.2222222222222222</v>
       </c>
       <c r="D30">
-        <v>-2.997305559944782</v>
+        <v>-2.980556322501973</v>
       </c>
       <c r="E30">
-        <v>-0.2139374910666447</v>
+        <v>-0.1971882536238345</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -913,10 +913,10 @@
         <v>0.2380952380952381</v>
       </c>
       <c r="D31">
-        <v>-2.97732201744751</v>
+        <v>-2.999703272438241</v>
       </c>
       <c r="E31">
-        <v>-0.1899839116536559</v>
+        <v>-0.2123651666443869</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -930,10 +930,10 @@
         <v>0.253968253968254</v>
       </c>
       <c r="D32">
-        <v>-3.021677260138665</v>
+        <v>-2.994606284722475</v>
       </c>
       <c r="E32">
-        <v>-0.2303691174290945</v>
+        <v>-0.2032981420129047</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -947,10 +947,10 @@
         <v>0.2698412698412698</v>
       </c>
       <c r="D33">
-        <v>-2.999017489587867</v>
+        <v>-3.009527842491398</v>
       </c>
       <c r="E33">
-        <v>-0.2037393099625797</v>
+        <v>-0.214249662866111</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -964,10 +964,10 @@
         <v>0.2857142857142857</v>
       </c>
       <c r="D34">
-        <v>-3.02569302077402</v>
+        <v>-3.028533220045101</v>
       </c>
       <c r="E34">
-        <v>-0.2264448042330165</v>
+        <v>-0.229285003504097</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -981,10 +981,10 @@
         <v>0.3015873015873016</v>
       </c>
       <c r="D35">
-        <v>-3.012119558849006</v>
+        <v>-3.019351713883343</v>
       </c>
       <c r="E35">
-        <v>-0.2089013053922857</v>
+        <v>-0.2161334604266232</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -998,10 +998,10 @@
         <v>0.3174603174603174</v>
       </c>
       <c r="D36">
-        <v>-3.087565474053564</v>
+        <v>-3.063362667386178</v>
       </c>
       <c r="E36">
-        <v>-0.2803771836811271</v>
+        <v>-0.256174377013741</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -1015,10 +1015,10 @@
         <v>0.3333333333333333</v>
       </c>
       <c r="D37">
-        <v>-3.110393467587341</v>
+        <v>-3.065829320437619</v>
       </c>
       <c r="E37">
-        <v>-0.2992351402991873</v>
+        <v>-0.2546709931494662</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -1032,10 +1032,10 @@
         <v>0.3492063492063492</v>
       </c>
       <c r="D38">
-        <v>-3.056519219041848</v>
+        <v>-3.037026970323365</v>
       </c>
       <c r="E38">
-        <v>-0.2413908548379782</v>
+        <v>-0.221898606119495</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -1049,10 +1049,10 @@
         <v>0.3650793650793651</v>
       </c>
       <c r="D39">
-        <v>-3.096976152836231</v>
+        <v>-3.081098662663362</v>
       </c>
       <c r="E39">
-        <v>-0.2778777517166451</v>
+        <v>-0.2620002615437762</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -1066,10 +1066,10 @@
         <v>0.3809523809523809</v>
       </c>
       <c r="D40">
-        <v>-3.051805770504576</v>
+        <v>-3.092065937571363</v>
       </c>
       <c r="E40">
-        <v>-0.2287373324692739</v>
+        <v>-0.2689974995360604</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -1083,10 +1083,10 @@
         <v>0.3968253968253968</v>
       </c>
       <c r="D41">
-        <v>-3.081707644236019</v>
+        <v>-3.073656185118655</v>
       </c>
       <c r="E41">
-        <v>-0.2546691692849989</v>
+        <v>-0.2466177101676352</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -1100,10 +1100,10 @@
         <v>0.4126984126984127</v>
       </c>
       <c r="D42">
-        <v>-3.074912184853791</v>
+        <v>-3.098541898095871</v>
       </c>
       <c r="E42">
-        <v>-0.243903672987055</v>
+        <v>-0.2675333862291356</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -1117,10 +1117,10 @@
         <v>0.4285714285714285</v>
       </c>
       <c r="D43">
-        <v>-3.112836332266358</v>
+        <v>-3.139479292821814</v>
       </c>
       <c r="E43">
-        <v>-0.2778577834839053</v>
+        <v>-0.3045007440393612</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -1134,10 +1134,10 @@
         <v>0.4444444444444444</v>
       </c>
       <c r="D44">
-        <v>-3.120892022743644</v>
+        <v>-3.153423368758159</v>
       </c>
       <c r="E44">
-        <v>-0.281943437045475</v>
+        <v>-0.3144747830599899</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -1151,10 +1151,10 @@
         <v>0.4603174603174603</v>
       </c>
       <c r="D45">
-        <v>-3.149975583337968</v>
+        <v>-3.119471255952907</v>
       </c>
       <c r="E45">
-        <v>-0.3070569607240827</v>
+        <v>-0.2765526333390218</v>
       </c>
     </row>
     <row r="46" spans="1:5">
@@ -1168,10 +1168,10 @@
         <v>0.4761904761904762</v>
       </c>
       <c r="D46">
-        <v>-3.141371871226871</v>
+        <v>-3.118665382102996</v>
       </c>
       <c r="E46">
-        <v>-0.2944832116972691</v>
+        <v>-0.271776722573394</v>
       </c>
     </row>
     <row r="47" spans="1:5">
@@ -1185,10 +1185,10 @@
         <v>0.492063492063492</v>
       </c>
       <c r="D47">
-        <v>-3.196435608425649</v>
+        <v>-3.146574918671662</v>
       </c>
       <c r="E47">
-        <v>-0.3455769119803305</v>
+        <v>-0.2957162222263434</v>
       </c>
     </row>
     <row r="48" spans="1:5">
@@ -1202,10 +1202,10 @@
         <v>0.5079365079365079</v>
       </c>
       <c r="D48">
-        <v>-3.122326868459893</v>
+        <v>-3.155541111546033</v>
       </c>
       <c r="E48">
-        <v>-0.2674981350988577</v>
+        <v>-0.3007123781849979</v>
       </c>
     </row>
     <row r="49" spans="1:5">
@@ -1219,10 +1219,10 @@
         <v>0.5238095238095238</v>
       </c>
       <c r="D49">
-        <v>-3.183660207758427</v>
+        <v>-3.135438621456831</v>
       </c>
       <c r="E49">
-        <v>-0.3248614374816756</v>
+        <v>-0.2766398511800796</v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -1236,10 +1236,10 @@
         <v>0.5396825396825397</v>
       </c>
       <c r="D50">
-        <v>-3.150731649537827</v>
+        <v>-3.186242417610071</v>
       </c>
       <c r="E50">
-        <v>-0.2879628423453591</v>
+        <v>-0.3234736104176026</v>
       </c>
     </row>
     <row r="51" spans="1:5">
@@ -1253,10 +1253,10 @@
         <v>0.5555555555555556</v>
       </c>
       <c r="D51">
-        <v>-3.198326892346483</v>
+        <v>-3.189446388069909</v>
       </c>
       <c r="E51">
-        <v>-0.3315880482382982</v>
+        <v>-0.3227075439617244</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -1270,10 +1270,10 @@
         <v>0.5714285714285714</v>
       </c>
       <c r="D52">
-        <v>-3.150337122526915</v>
+        <v>-3.182553760843985</v>
       </c>
       <c r="E52">
-        <v>-0.2796282415030138</v>
+        <v>-0.3118448798200841</v>
       </c>
     </row>
     <row r="53" spans="1:5">
@@ -1287,10 +1287,10 @@
         <v>0.5873015873015873</v>
       </c>
       <c r="D53">
-        <v>-3.15705558337584</v>
+        <v>-3.175541855519404</v>
       </c>
       <c r="E53">
-        <v>-0.2823766654362223</v>
+        <v>-0.3008629375797867</v>
       </c>
     </row>
     <row r="54" spans="1:5">
@@ -1304,10 +1304,10 @@
         <v>0.6031746031746031</v>
       </c>
       <c r="D54">
-        <v>-3.149128429465391</v>
+        <v>-3.1905979654172</v>
       </c>
       <c r="E54">
-        <v>-0.2704794746100565</v>
+        <v>-0.3119490105618659</v>
       </c>
     </row>
     <row r="55" spans="1:5">
@@ -1321,10 +1321,10 @@
         <v>0.6190476190476191</v>
       </c>
       <c r="D55">
-        <v>-3.152100323990135</v>
+        <v>-3.133254836413261</v>
       </c>
       <c r="E55">
-        <v>-0.2694813322190843</v>
+        <v>-0.2506358446422106</v>
       </c>
     </row>
     <row r="56" spans="1:5">
@@ -1338,10 +1338,10 @@
         <v>0.6349206349206349</v>
       </c>
       <c r="D56">
-        <v>-3.125574613610699</v>
+        <v>-3.176800618940493</v>
       </c>
       <c r="E56">
-        <v>-0.2389855849239324</v>
+        <v>-0.2902115902537257</v>
       </c>
     </row>
     <row r="57" spans="1:5">
@@ -1355,10 +1355,10 @@
         <v>0.6507936507936508</v>
       </c>
       <c r="D57">
-        <v>-3.177992412723909</v>
+        <v>-3.176841089972586</v>
       </c>
       <c r="E57">
-        <v>-0.2874333471214259</v>
+        <v>-0.2862820243701023</v>
       </c>
     </row>
     <row r="58" spans="1:5">
@@ -1372,10 +1372,10 @@
         <v>0.6666666666666666</v>
       </c>
       <c r="D58">
-        <v>-3.152864259362092</v>
+        <v>-3.175976411261993</v>
       </c>
       <c r="E58">
-        <v>-0.2583351568438919</v>
+        <v>-0.2814473087437932</v>
       </c>
     </row>
     <row r="59" spans="1:5">
@@ -1389,10 +1389,10 @@
         <v>0.6825396825396826</v>
       </c>
       <c r="D59">
-        <v>-3.162784989612202</v>
+        <v>-3.145337328302018</v>
       </c>
       <c r="E59">
-        <v>-0.2642858501782859</v>
+        <v>-0.2468381888681017</v>
       </c>
     </row>
     <row r="60" spans="1:5">
@@ -1406,10 +1406,10 @@
         <v>0.6984126984126984</v>
       </c>
       <c r="D60">
-        <v>-3.164106160337457</v>
+        <v>-3.163976783395619</v>
       </c>
       <c r="E60">
-        <v>-0.2616369839878242</v>
+        <v>-0.2615076070459857</v>
       </c>
     </row>
     <row r="61" spans="1:5">
@@ -1423,10 +1423,10 @@
         <v>0.7142857142857143</v>
       </c>
       <c r="D61">
-        <v>-3.157718460003845</v>
+        <v>-3.139624402834649</v>
       </c>
       <c r="E61">
-        <v>-0.2512792467384956</v>
+        <v>-0.2331851895692995</v>
       </c>
     </row>
     <row r="62" spans="1:5">
@@ -1440,10 +1440,10 @@
         <v>0.7301587301587301</v>
       </c>
       <c r="D62">
-        <v>-3.148135056449763</v>
+        <v>-3.14761803753259</v>
       </c>
       <c r="E62">
-        <v>-0.237725806268697</v>
+        <v>-0.2372087873515235</v>
       </c>
     </row>
     <row r="63" spans="1:5">
@@ -1457,10 +1457,10 @@
         <v>0.746031746031746</v>
       </c>
       <c r="D63">
-        <v>-3.150736926868178</v>
+        <v>-3.139574087555343</v>
       </c>
       <c r="E63">
-        <v>-0.2363576397713955</v>
+        <v>-0.2251948004585606</v>
       </c>
     </row>
     <row r="64" spans="1:5">
@@ -1474,10 +1474,10 @@
         <v>0.7619047619047619</v>
       </c>
       <c r="D64">
-        <v>-3.135242859715741</v>
+        <v>-3.136523559408903</v>
       </c>
       <c r="E64">
-        <v>-0.2168935357032418</v>
+        <v>-0.2181742353964038</v>
       </c>
     </row>
     <row r="65" spans="1:5">
@@ -1491,10 +1491,10 @@
         <v>0.7777777777777778</v>
       </c>
       <c r="D65">
-        <v>-3.134119427121472</v>
+        <v>-3.129372178299302</v>
       </c>
       <c r="E65">
-        <v>-0.2118000661932558</v>
+        <v>-0.2070528173710866</v>
       </c>
     </row>
     <row r="66" spans="1:5">
@@ -1508,10 +1508,10 @@
         <v>0.7936507936507936</v>
       </c>
       <c r="D66">
-        <v>-3.120811209404883</v>
+        <v>-3.125170327401539</v>
       </c>
       <c r="E66">
-        <v>-0.1945218115609503</v>
+        <v>-0.1988809295576067</v>
       </c>
     </row>
     <row r="67" spans="1:5">
@@ -1525,10 +1525,10 @@
         <v>0.8095238095238095</v>
       </c>
       <c r="D67">
-        <v>-3.123671344856795</v>
+        <v>-3.118407077117454</v>
       </c>
       <c r="E67">
-        <v>-0.1934119100971466</v>
+        <v>-0.1881476423578049</v>
       </c>
     </row>
     <row r="68" spans="1:5">
@@ -1542,10 +1542,10 @@
         <v>0.8253968253968254</v>
       </c>
       <c r="D68">
-        <v>-3.107025954953035</v>
+        <v>-3.107025954953037</v>
       </c>
       <c r="E68">
-        <v>-0.1727964832776704</v>
+        <v>-0.1727964832776717</v>
       </c>
     </row>
     <row r="69" spans="1:5">
@@ -1559,10 +1559,10 @@
         <v>0.8412698412698413</v>
       </c>
       <c r="D69">
-        <v>-3.098852628033951</v>
+        <v>-3.104492445723768</v>
       </c>
       <c r="E69">
-        <v>-0.160653119442869</v>
+        <v>-0.1662929371326861</v>
       </c>
     </row>
     <row r="70" spans="1:5">
@@ -1576,10 +1576,10 @@
         <v>0.8571428571428571</v>
       </c>
       <c r="D70">
-        <v>-3.094392023252511</v>
+        <v>-3.089903528314018</v>
       </c>
       <c r="E70">
-        <v>-0.1522224777457127</v>
+        <v>-0.1477339828072196</v>
       </c>
     </row>
     <row r="71" spans="1:5">
@@ -1593,10 +1593,10 @@
         <v>0.873015873015873</v>
       </c>
       <c r="D71">
-        <v>-3.083010901088094</v>
+        <v>-3.083010901088095</v>
       </c>
       <c r="E71">
-        <v>-0.1368713186655793</v>
+        <v>-0.1368713186655797</v>
       </c>
     </row>
     <row r="72" spans="1:5">
@@ -1610,10 +1610,10 @@
         <v>0.8888888888888888</v>
       </c>
       <c r="D72">
-        <v>-3.070478456172353</v>
+        <v>-3.070478456172355</v>
       </c>
       <c r="E72">
-        <v>-0.120368836834122</v>
+        <v>-0.1203688368341242</v>
       </c>
     </row>
     <row r="73" spans="1:5">
@@ -1627,10 +1627,10 @@
         <v>0.9047619047619048</v>
       </c>
       <c r="D73">
-        <v>-3.057946011256614</v>
+        <v>-3.057946011256613</v>
       </c>
       <c r="E73">
-        <v>-0.1038663550026659</v>
+        <v>-0.1038663550026654</v>
       </c>
     </row>
     <row r="74" spans="1:5">
@@ -1644,10 +1644,10 @@
         <v>0.9206349206349206</v>
       </c>
       <c r="D74">
-        <v>-3.049772684337529</v>
+        <v>-3.048621361586205</v>
       </c>
       <c r="E74">
-        <v>-0.09172299116786464</v>
+        <v>-0.09057166841654107</v>
       </c>
     </row>
     <row r="75" spans="1:5">
@@ -1661,10 +1661,10 @@
         <v>0.9365079365079365</v>
       </c>
       <c r="D75">
-        <v>-3.036088916670467</v>
+        <v>-3.037240239421788</v>
       </c>
       <c r="E75">
-        <v>-0.07406918658508591</v>
+        <v>-0.0752205093364077</v>
       </c>
     </row>
     <row r="76" spans="1:5">
@@ -1681,7 +1681,7 @@
         <v>-3.022405149003403</v>
       </c>
       <c r="E76">
-        <v>-0.0564153820023055</v>
+        <v>-0.05641538200230595</v>
       </c>
     </row>
     <row r="77" spans="1:5">
@@ -1732,6 +1732,1876 @@
         <v>-2.977899877748247</v>
       </c>
       <c r="E79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5">
+      <c r="A80">
+        <v>171</v>
+      </c>
+      <c r="B80">
+        <v>1.083</v>
+      </c>
+      <c r="C80">
+        <v>0</v>
+      </c>
+      <c r="D80">
+        <v>-2.959880304825162</v>
+      </c>
+      <c r="E80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5">
+      <c r="A81">
+        <v>171</v>
+      </c>
+      <c r="B81">
+        <v>1.083</v>
+      </c>
+      <c r="C81">
+        <v>0.1</v>
+      </c>
+      <c r="D81">
+        <v>-3.058356608783145</v>
+      </c>
+      <c r="E81">
+        <v>-0.07133700030342593</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5">
+      <c r="A82">
+        <v>171</v>
+      </c>
+      <c r="B82">
+        <v>1.083</v>
+      </c>
+      <c r="C82">
+        <v>0.2</v>
+      </c>
+      <c r="D82">
+        <v>-3.135725781470565</v>
+      </c>
+      <c r="E82">
+        <v>-0.1215668693362884</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5">
+      <c r="A83">
+        <v>171</v>
+      </c>
+      <c r="B83">
+        <v>1.083</v>
+      </c>
+      <c r="C83">
+        <v>0.3</v>
+      </c>
+      <c r="D83">
+        <v>-3.192583078351433</v>
+      </c>
+      <c r="E83">
+        <v>-0.1512848625625987</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5">
+      <c r="A84">
+        <v>171</v>
+      </c>
+      <c r="B84">
+        <v>1.083</v>
+      </c>
+      <c r="C84">
+        <v>0.4</v>
+      </c>
+      <c r="D84">
+        <v>-3.254713279152627</v>
+      </c>
+      <c r="E84">
+        <v>-0.186275759709235</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5">
+      <c r="A85">
+        <v>171</v>
+      </c>
+      <c r="B85">
+        <v>1.083</v>
+      </c>
+      <c r="C85">
+        <v>0.5</v>
+      </c>
+      <c r="D85">
+        <v>-3.306201424589144</v>
+      </c>
+      <c r="E85">
+        <v>-0.2106246014911946</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5">
+      <c r="A86">
+        <v>171</v>
+      </c>
+      <c r="B86">
+        <v>1.083</v>
+      </c>
+      <c r="C86">
+        <v>0.6000000000000001</v>
+      </c>
+      <c r="D86">
+        <v>-3.320452310899221</v>
+      </c>
+      <c r="E86">
+        <v>-0.1977361841467136</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5">
+      <c r="A87">
+        <v>171</v>
+      </c>
+      <c r="B87">
+        <v>1.083</v>
+      </c>
+      <c r="C87">
+        <v>0.7000000000000001</v>
+      </c>
+      <c r="D87">
+        <v>-3.329520207746302</v>
+      </c>
+      <c r="E87">
+        <v>-0.1796647773392374</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5">
+      <c r="A88">
+        <v>171</v>
+      </c>
+      <c r="B88">
+        <v>1.083</v>
+      </c>
+      <c r="C88">
+        <v>0.8</v>
+      </c>
+      <c r="D88">
+        <v>-3.35077729546683</v>
+      </c>
+      <c r="E88">
+        <v>-0.1737825614052075</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5">
+      <c r="A89">
+        <v>171</v>
+      </c>
+      <c r="B89">
+        <v>1.083</v>
+      </c>
+      <c r="C89">
+        <v>0.9</v>
+      </c>
+      <c r="D89">
+        <v>-3.318157016472849</v>
+      </c>
+      <c r="E89">
+        <v>-0.1140229787566692</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5">
+      <c r="A90">
+        <v>171</v>
+      </c>
+      <c r="B90">
+        <v>1.083</v>
+      </c>
+      <c r="C90">
+        <v>1</v>
+      </c>
+      <c r="D90">
+        <v>-3.231273341370737</v>
+      </c>
+      <c r="E90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5">
+      <c r="A91">
+        <v>365</v>
+      </c>
+      <c r="B91">
+        <v>1.444</v>
+      </c>
+      <c r="C91">
+        <v>0</v>
+      </c>
+      <c r="D91">
+        <v>-3.066537620233559</v>
+      </c>
+      <c r="E91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5">
+      <c r="A92">
+        <v>365</v>
+      </c>
+      <c r="B92">
+        <v>1.444</v>
+      </c>
+      <c r="C92">
+        <v>0.1</v>
+      </c>
+      <c r="D92">
+        <v>-3.161581195732908</v>
+      </c>
+      <c r="E92">
+        <v>-0.06692632511325503</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5">
+      <c r="A93">
+        <v>365</v>
+      </c>
+      <c r="B93">
+        <v>1.444</v>
+      </c>
+      <c r="C93">
+        <v>0.2</v>
+      </c>
+      <c r="D93">
+        <v>-3.236372728691916</v>
+      </c>
+      <c r="E93">
+        <v>-0.1136006076861698</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5">
+      <c r="A94">
+        <v>365</v>
+      </c>
+      <c r="B94">
+        <v>1.444</v>
+      </c>
+      <c r="C94">
+        <v>0.3</v>
+      </c>
+      <c r="D94">
+        <v>-3.288338270252288</v>
+      </c>
+      <c r="E94">
+        <v>-0.1374488988604488</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5">
+      <c r="A95">
+        <v>365</v>
+      </c>
+      <c r="B95">
+        <v>1.444</v>
+      </c>
+      <c r="C95">
+        <v>0.4</v>
+      </c>
+      <c r="D95">
+        <v>-3.354550452239324</v>
+      </c>
+      <c r="E95">
+        <v>-0.1755438304613919</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5">
+      <c r="A96">
+        <v>365</v>
+      </c>
+      <c r="B96">
+        <v>1.444</v>
+      </c>
+      <c r="C96">
+        <v>0.5</v>
+      </c>
+      <c r="D96">
+        <v>-3.384297884273012</v>
+      </c>
+      <c r="E96">
+        <v>-0.1771740121089866</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5">
+      <c r="A97">
+        <v>365</v>
+      </c>
+      <c r="B97">
+        <v>1.444</v>
+      </c>
+      <c r="C97">
+        <v>0.6000000000000001</v>
+      </c>
+      <c r="D97">
+        <v>-3.407656001362706</v>
+      </c>
+      <c r="E97">
+        <v>-0.172414878812587</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5">
+      <c r="A98">
+        <v>365</v>
+      </c>
+      <c r="B98">
+        <v>1.444</v>
+      </c>
+      <c r="C98">
+        <v>0.7000000000000001</v>
+      </c>
+      <c r="D98">
+        <v>-3.425750486464414</v>
+      </c>
+      <c r="E98">
+        <v>-0.1623921135282019</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5">
+      <c r="A99">
+        <v>365</v>
+      </c>
+      <c r="B99">
+        <v>1.444</v>
+      </c>
+      <c r="C99">
+        <v>0.8</v>
+      </c>
+      <c r="D99">
+        <v>-3.424499944765616</v>
+      </c>
+      <c r="E99">
+        <v>-0.1330243214433109</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5">
+      <c r="A100">
+        <v>365</v>
+      </c>
+      <c r="B100">
+        <v>1.444</v>
+      </c>
+      <c r="C100">
+        <v>0.9</v>
+      </c>
+      <c r="D100">
+        <v>-3.413115677387186</v>
+      </c>
+      <c r="E100">
+        <v>-0.09352280367878718</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5">
+      <c r="A101">
+        <v>365</v>
+      </c>
+      <c r="B101">
+        <v>1.444</v>
+      </c>
+      <c r="C101">
+        <v>1</v>
+      </c>
+      <c r="D101">
+        <v>-3.347710124094492</v>
+      </c>
+      <c r="E101">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5">
+      <c r="A102">
+        <v>665</v>
+      </c>
+      <c r="B102">
+        <v>1.805</v>
+      </c>
+      <c r="C102">
+        <v>0</v>
+      </c>
+      <c r="D102">
+        <v>-3.147240082658214</v>
+      </c>
+      <c r="E102">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5">
+      <c r="A103">
+        <v>665</v>
+      </c>
+      <c r="B103">
+        <v>1.805</v>
+      </c>
+      <c r="C103">
+        <v>0.1</v>
+      </c>
+      <c r="D103">
+        <v>-3.233096084150288</v>
+      </c>
+      <c r="E103">
+        <v>-0.05699878583446827</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5">
+      <c r="A104">
+        <v>665</v>
+      </c>
+      <c r="B104">
+        <v>1.805</v>
+      </c>
+      <c r="C104">
+        <v>0.2</v>
+      </c>
+      <c r="D104">
+        <v>-3.304764538410597</v>
+      </c>
+      <c r="E104">
+        <v>-0.0998100244371698</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5">
+      <c r="A105">
+        <v>665</v>
+      </c>
+      <c r="B105">
+        <v>1.805</v>
+      </c>
+      <c r="C105">
+        <v>0.3</v>
+      </c>
+      <c r="D105">
+        <v>-3.360443864832046</v>
+      </c>
+      <c r="E105">
+        <v>-0.1266321352010125</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5">
+      <c r="A106">
+        <v>665</v>
+      </c>
+      <c r="B106">
+        <v>1.805</v>
+      </c>
+      <c r="C106">
+        <v>0.4</v>
+      </c>
+      <c r="D106">
+        <v>-3.403472159370311</v>
+      </c>
+      <c r="E106">
+        <v>-0.1408032140816711</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5">
+      <c r="A107">
+        <v>665</v>
+      </c>
+      <c r="B107">
+        <v>1.805</v>
+      </c>
+      <c r="C107">
+        <v>0.5</v>
+      </c>
+      <c r="D107">
+        <v>-3.441249060163437</v>
+      </c>
+      <c r="E107">
+        <v>-0.1497228992171906</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5">
+      <c r="A108">
+        <v>665</v>
+      </c>
+      <c r="B108">
+        <v>1.805</v>
+      </c>
+      <c r="C108">
+        <v>0.6000000000000001</v>
+      </c>
+      <c r="D108">
+        <v>-3.464903714971963</v>
+      </c>
+      <c r="E108">
+        <v>-0.1445203383681097</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5">
+      <c r="A109">
+        <v>665</v>
+      </c>
+      <c r="B109">
+        <v>1.805</v>
+      </c>
+      <c r="C109">
+        <v>0.7000000000000001</v>
+      </c>
+      <c r="D109">
+        <v>-3.476534904753164</v>
+      </c>
+      <c r="E109">
+        <v>-0.1272943124917048</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5">
+      <c r="A110">
+        <v>665</v>
+      </c>
+      <c r="B110">
+        <v>1.805</v>
+      </c>
+      <c r="C110">
+        <v>0.8</v>
+      </c>
+      <c r="D110">
+        <v>-3.487543401036584</v>
+      </c>
+      <c r="E110">
+        <v>-0.1094455931175183</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5">
+      <c r="A111">
+        <v>665</v>
+      </c>
+      <c r="B111">
+        <v>1.805</v>
+      </c>
+      <c r="C111">
+        <v>0.9</v>
+      </c>
+      <c r="D111">
+        <v>-3.477519463532454</v>
+      </c>
+      <c r="E111">
+        <v>-0.07056443995578171</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5">
+      <c r="A112">
+        <v>665</v>
+      </c>
+      <c r="B112">
+        <v>1.805</v>
+      </c>
+      <c r="C112">
+        <v>1</v>
+      </c>
+      <c r="D112">
+        <v>-3.435812239234279</v>
+      </c>
+      <c r="E112">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5">
+      <c r="A113">
+        <v>1099</v>
+      </c>
+      <c r="B113">
+        <v>2.166</v>
+      </c>
+      <c r="C113">
+        <v>0</v>
+      </c>
+      <c r="D113">
+        <v>-3.196470301605819</v>
+      </c>
+      <c r="E113">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5">
+      <c r="A114">
+        <v>1099</v>
+      </c>
+      <c r="B114">
+        <v>2.166</v>
+      </c>
+      <c r="C114">
+        <v>0.1</v>
+      </c>
+      <c r="D114">
+        <v>-3.279642334612179</v>
+      </c>
+      <c r="E114">
+        <v>-0.05386342279105838</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5">
+      <c r="A115">
+        <v>1099</v>
+      </c>
+      <c r="B115">
+        <v>2.166</v>
+      </c>
+      <c r="C115">
+        <v>0.2</v>
+      </c>
+      <c r="D115">
+        <v>-3.344053583592614</v>
+      </c>
+      <c r="E115">
+        <v>-0.08896606155619136</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5">
+      <c r="A116">
+        <v>1099</v>
+      </c>
+      <c r="B116">
+        <v>2.166</v>
+      </c>
+      <c r="C116">
+        <v>0.3</v>
+      </c>
+      <c r="D116">
+        <v>-3.394086560507519</v>
+      </c>
+      <c r="E116">
+        <v>-0.1096904282557944</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5">
+      <c r="A117">
+        <v>1099</v>
+      </c>
+      <c r="B117">
+        <v>2.166</v>
+      </c>
+      <c r="C117">
+        <v>0.4</v>
+      </c>
+      <c r="D117">
+        <v>-3.444413412094474</v>
+      </c>
+      <c r="E117">
+        <v>-0.1307086696274469</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5">
+      <c r="A118">
+        <v>1099</v>
+      </c>
+      <c r="B118">
+        <v>2.166</v>
+      </c>
+      <c r="C118">
+        <v>0.5</v>
+      </c>
+      <c r="D118">
+        <v>-3.480654289073926</v>
+      </c>
+      <c r="E118">
+        <v>-0.1376409363915967</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5">
+      <c r="A119">
+        <v>1099</v>
+      </c>
+      <c r="B119">
+        <v>2.166</v>
+      </c>
+      <c r="C119">
+        <v>0.6000000000000001</v>
+      </c>
+      <c r="D119">
+        <v>-3.500354909432203</v>
+      </c>
+      <c r="E119">
+        <v>-0.1280329465345722</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5">
+      <c r="A120">
+        <v>1099</v>
+      </c>
+      <c r="B120">
+        <v>2.166</v>
+      </c>
+      <c r="C120">
+        <v>0.7000000000000001</v>
+      </c>
+      <c r="D120">
+        <v>-3.515197055561998</v>
+      </c>
+      <c r="E120">
+        <v>-0.1135664824490653</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5">
+      <c r="A121">
+        <v>1099</v>
+      </c>
+      <c r="B121">
+        <v>2.166</v>
+      </c>
+      <c r="C121">
+        <v>0.8</v>
+      </c>
+      <c r="D121">
+        <v>-3.522287844998943</v>
+      </c>
+      <c r="E121">
+        <v>-0.09134866167070799</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5">
+      <c r="A122">
+        <v>1099</v>
+      </c>
+      <c r="B122">
+        <v>2.166</v>
+      </c>
+      <c r="C122">
+        <v>0.9</v>
+      </c>
+      <c r="D122">
+        <v>-3.521505561845264</v>
+      </c>
+      <c r="E122">
+        <v>-0.06125776830172747</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5">
+      <c r="A123">
+        <v>1099</v>
+      </c>
+      <c r="B123">
+        <v>2.166</v>
+      </c>
+      <c r="C123">
+        <v>1</v>
+      </c>
+      <c r="D123">
+        <v>-3.489556403758839</v>
+      </c>
+      <c r="E123">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5">
+      <c r="A124">
+        <v>1687</v>
+      </c>
+      <c r="B124">
+        <v>2.527</v>
+      </c>
+      <c r="C124">
+        <v>0</v>
+      </c>
+      <c r="D124">
+        <v>-3.237065081377683</v>
+      </c>
+      <c r="E124">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5">
+      <c r="A125">
+        <v>1687</v>
+      </c>
+      <c r="B125">
+        <v>2.527</v>
+      </c>
+      <c r="C125">
+        <v>0.1</v>
+      </c>
+      <c r="D125">
+        <v>-3.314745822582975</v>
+      </c>
+      <c r="E125">
+        <v>-0.04799991524422165</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5">
+      <c r="A126">
+        <v>1687</v>
+      </c>
+      <c r="B126">
+        <v>2.527</v>
+      </c>
+      <c r="C126">
+        <v>0.2</v>
+      </c>
+      <c r="D126">
+        <v>-3.377927488883896</v>
+      </c>
+      <c r="E126">
+        <v>-0.08150075558407144</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5">
+      <c r="A127">
+        <v>1687</v>
+      </c>
+      <c r="B127">
+        <v>2.527</v>
+      </c>
+      <c r="C127">
+        <v>0.3</v>
+      </c>
+      <c r="D127">
+        <v>-3.431028964847889</v>
+      </c>
+      <c r="E127">
+        <v>-0.1049214055869938</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5">
+      <c r="A128">
+        <v>1687</v>
+      </c>
+      <c r="B128">
+        <v>2.527</v>
+      </c>
+      <c r="C128">
+        <v>0.4</v>
+      </c>
+      <c r="D128">
+        <v>-3.475518749631872</v>
+      </c>
+      <c r="E128">
+        <v>-0.1197303644099061</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5">
+      <c r="A129">
+        <v>1687</v>
+      </c>
+      <c r="B129">
+        <v>2.527</v>
+      </c>
+      <c r="C129">
+        <v>0.5</v>
+      </c>
+      <c r="D129">
+        <v>-3.506959582804033</v>
+      </c>
+      <c r="E129">
+        <v>-0.1214903716209965</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5">
+      <c r="A130">
+        <v>1687</v>
+      </c>
+      <c r="B130">
+        <v>2.527</v>
+      </c>
+      <c r="C130">
+        <v>0.6000000000000001</v>
+      </c>
+      <c r="D130">
+        <v>-3.535781107116629</v>
+      </c>
+      <c r="E130">
+        <v>-0.1206310699725217</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5">
+      <c r="A131">
+        <v>1687</v>
+      </c>
+      <c r="B131">
+        <v>2.527</v>
+      </c>
+      <c r="C131">
+        <v>0.7000000000000001</v>
+      </c>
+      <c r="D131">
+        <v>-3.553393583412525</v>
+      </c>
+      <c r="E131">
+        <v>-0.1085627203073463</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5">
+      <c r="A132">
+        <v>1687</v>
+      </c>
+      <c r="B132">
+        <v>2.527</v>
+      </c>
+      <c r="C132">
+        <v>0.8</v>
+      </c>
+      <c r="D132">
+        <v>-3.562021687351217</v>
+      </c>
+      <c r="E132">
+        <v>-0.08750999828496775</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5">
+      <c r="A133">
+        <v>1687</v>
+      </c>
+      <c r="B133">
+        <v>2.527</v>
+      </c>
+      <c r="C133">
+        <v>0.9</v>
+      </c>
+      <c r="D133">
+        <v>-3.56071317867139</v>
+      </c>
+      <c r="E133">
+        <v>-0.05652066364407043</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5">
+      <c r="A134">
+        <v>1687</v>
+      </c>
+      <c r="B134">
+        <v>2.527</v>
+      </c>
+      <c r="C134">
+        <v>1</v>
+      </c>
+      <c r="D134">
+        <v>-3.533873340988391</v>
+      </c>
+      <c r="E134">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5">
+      <c r="A135">
+        <v>2457</v>
+      </c>
+      <c r="B135">
+        <v>2.888</v>
+      </c>
+      <c r="C135">
+        <v>0</v>
+      </c>
+      <c r="D135">
+        <v>-3.265296909246303</v>
+      </c>
+      <c r="E135">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5">
+      <c r="A136">
+        <v>2457</v>
+      </c>
+      <c r="B136">
+        <v>2.888</v>
+      </c>
+      <c r="C136">
+        <v>0.1</v>
+      </c>
+      <c r="D136">
+        <v>-3.342018340796063</v>
+      </c>
+      <c r="E136">
+        <v>-0.04678174642197153</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5">
+      <c r="A137">
+        <v>2457</v>
+      </c>
+      <c r="B137">
+        <v>2.888</v>
+      </c>
+      <c r="C137">
+        <v>0.2</v>
+      </c>
+      <c r="D137">
+        <v>-3.40215548275237</v>
+      </c>
+      <c r="E137">
+        <v>-0.0769792032504899</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5">
+      <c r="A138">
+        <v>2457</v>
+      </c>
+      <c r="B138">
+        <v>2.888</v>
+      </c>
+      <c r="C138">
+        <v>0.3</v>
+      </c>
+      <c r="D138">
+        <v>-3.456100152157441</v>
+      </c>
+      <c r="E138">
+        <v>-0.1009841875277733</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5">
+      <c r="A139">
+        <v>2457</v>
+      </c>
+      <c r="B139">
+        <v>2.888</v>
+      </c>
+      <c r="C139">
+        <v>0.4</v>
+      </c>
+      <c r="D139">
+        <v>-3.499380358962707</v>
+      </c>
+      <c r="E139">
+        <v>-0.1143247092052506</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5">
+      <c r="A140">
+        <v>2457</v>
+      </c>
+      <c r="B140">
+        <v>2.888</v>
+      </c>
+      <c r="C140">
+        <v>0.5</v>
+      </c>
+      <c r="D140">
+        <v>-3.534958005770232</v>
+      </c>
+      <c r="E140">
+        <v>-0.119962670884987</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5">
+      <c r="A141">
+        <v>2457</v>
+      </c>
+      <c r="B141">
+        <v>2.888</v>
+      </c>
+      <c r="C141">
+        <v>0.6000000000000001</v>
+      </c>
+      <c r="D141">
+        <v>-3.559010414775953</v>
+      </c>
+      <c r="E141">
+        <v>-0.1140753947629201</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5">
+      <c r="A142">
+        <v>2457</v>
+      </c>
+      <c r="B142">
+        <v>2.888</v>
+      </c>
+      <c r="C142">
+        <v>0.7000000000000001</v>
+      </c>
+      <c r="D142">
+        <v>-3.578640233582048</v>
+      </c>
+      <c r="E142">
+        <v>-0.1037655284412266</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5">
+      <c r="A143">
+        <v>2457</v>
+      </c>
+      <c r="B143">
+        <v>2.888</v>
+      </c>
+      <c r="C143">
+        <v>0.8</v>
+      </c>
+      <c r="D143">
+        <v>-3.585101801018822</v>
+      </c>
+      <c r="E143">
+        <v>-0.08028741075021195</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5">
+      <c r="A144">
+        <v>2457</v>
+      </c>
+      <c r="B144">
+        <v>2.888</v>
+      </c>
+      <c r="C144">
+        <v>0.9</v>
+      </c>
+      <c r="D144">
+        <v>-3.58303208388604</v>
+      </c>
+      <c r="E144">
+        <v>-0.04827800848964131</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5">
+      <c r="A145">
+        <v>2457</v>
+      </c>
+      <c r="B145">
+        <v>2.888</v>
+      </c>
+      <c r="C145">
+        <v>1</v>
+      </c>
+      <c r="D145">
+        <v>-3.564693760524187</v>
+      </c>
+      <c r="E145">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5">
+      <c r="A146">
+        <v>3429</v>
+      </c>
+      <c r="B146">
+        <v>3.249</v>
+      </c>
+      <c r="C146">
+        <v>0</v>
+      </c>
+      <c r="D146">
+        <v>-3.289665192206087</v>
+      </c>
+      <c r="E146">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5">
+      <c r="A147">
+        <v>3429</v>
+      </c>
+      <c r="B147">
+        <v>3.249</v>
+      </c>
+      <c r="C147">
+        <v>0.1</v>
+      </c>
+      <c r="D147">
+        <v>-3.364323948766299</v>
+      </c>
+      <c r="E147">
+        <v>-0.04449563731934081</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5">
+      <c r="A148">
+        <v>3429</v>
+      </c>
+      <c r="B148">
+        <v>3.249</v>
+      </c>
+      <c r="C148">
+        <v>0.2</v>
+      </c>
+      <c r="D148">
+        <v>-3.424525887254642</v>
+      </c>
+      <c r="E148">
+        <v>-0.07453445656681357</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5">
+      <c r="A149">
+        <v>3429</v>
+      </c>
+      <c r="B149">
+        <v>3.249</v>
+      </c>
+      <c r="C149">
+        <v>0.3</v>
+      </c>
+      <c r="D149">
+        <v>-3.477855097229322</v>
+      </c>
+      <c r="E149">
+        <v>-0.09770054730062272</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5">
+      <c r="A150">
+        <v>3429</v>
+      </c>
+      <c r="B150">
+        <v>3.249</v>
+      </c>
+      <c r="C150">
+        <v>0.4</v>
+      </c>
+      <c r="D150">
+        <v>-3.522939214065749</v>
+      </c>
+      <c r="E150">
+        <v>-0.1126215448961794</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5">
+      <c r="A151">
+        <v>3429</v>
+      </c>
+      <c r="B151">
+        <v>3.249</v>
+      </c>
+      <c r="C151">
+        <v>0.5</v>
+      </c>
+      <c r="D151">
+        <v>-3.556009560925981</v>
+      </c>
+      <c r="E151">
+        <v>-0.1155287725155412</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5">
+      <c r="A152">
+        <v>3429</v>
+      </c>
+      <c r="B152">
+        <v>3.249</v>
+      </c>
+      <c r="C152">
+        <v>0.6000000000000001</v>
+      </c>
+      <c r="D152">
+        <v>-3.58246111752868</v>
+      </c>
+      <c r="E152">
+        <v>-0.1118172098773693</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5">
+      <c r="A153">
+        <v>3429</v>
+      </c>
+      <c r="B153">
+        <v>3.249</v>
+      </c>
+      <c r="C153">
+        <v>0.7000000000000001</v>
+      </c>
+      <c r="D153">
+        <v>-3.600001081311948</v>
+      </c>
+      <c r="E153">
+        <v>-0.09919405441976648</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5">
+      <c r="A154">
+        <v>3429</v>
+      </c>
+      <c r="B154">
+        <v>3.249</v>
+      </c>
+      <c r="C154">
+        <v>0.8</v>
+      </c>
+      <c r="D154">
+        <v>-3.608271653611407</v>
+      </c>
+      <c r="E154">
+        <v>-0.07730150747835596</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5">
+      <c r="A155">
+        <v>3429</v>
+      </c>
+      <c r="B155">
+        <v>3.249</v>
+      </c>
+      <c r="C155">
+        <v>0.9</v>
+      </c>
+      <c r="D155">
+        <v>-3.610087355988972</v>
+      </c>
+      <c r="E155">
+        <v>-0.04895409061504935</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5">
+      <c r="A156">
+        <v>3429</v>
+      </c>
+      <c r="B156">
+        <v>3.249</v>
+      </c>
+      <c r="C156">
+        <v>1</v>
+      </c>
+      <c r="D156">
+        <v>-3.591296384614793</v>
+      </c>
+      <c r="E156">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5">
+      <c r="A157">
+        <v>4631</v>
+      </c>
+      <c r="B157">
+        <v>3.61</v>
+      </c>
+      <c r="C157">
+        <v>0</v>
+      </c>
+      <c r="D157">
+        <v>-3.307947995043365</v>
+      </c>
+      <c r="E157">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5">
+      <c r="A158">
+        <v>4631</v>
+      </c>
+      <c r="B158">
+        <v>3.61</v>
+      </c>
+      <c r="C158">
+        <v>0.1</v>
+      </c>
+      <c r="D158">
+        <v>-3.381484449756316</v>
+      </c>
+      <c r="E158">
+        <v>-0.04320569945753716</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5">
+      <c r="A159">
+        <v>4631</v>
+      </c>
+      <c r="B159">
+        <v>3.61</v>
+      </c>
+      <c r="C159">
+        <v>0.2</v>
+      </c>
+      <c r="D159">
+        <v>-3.442508782265875</v>
+      </c>
+      <c r="E159">
+        <v>-0.07389927671168239</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5">
+      <c r="A160">
+        <v>4631</v>
+      </c>
+      <c r="B160">
+        <v>3.61</v>
+      </c>
+      <c r="C160">
+        <v>0.3</v>
+      </c>
+      <c r="D160">
+        <v>-3.493856201376004</v>
+      </c>
+      <c r="E160">
+        <v>-0.09491594056639796</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5">
+      <c r="A161">
+        <v>4631</v>
+      </c>
+      <c r="B161">
+        <v>3.61</v>
+      </c>
+      <c r="C161">
+        <v>0.4</v>
+      </c>
+      <c r="D161">
+        <v>-3.536289868406675</v>
+      </c>
+      <c r="E161">
+        <v>-0.1070188523416555</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5">
+      <c r="A162">
+        <v>4631</v>
+      </c>
+      <c r="B162">
+        <v>3.61</v>
+      </c>
+      <c r="C162">
+        <v>0.5</v>
+      </c>
+      <c r="D162">
+        <v>-3.571341619483734</v>
+      </c>
+      <c r="E162">
+        <v>-0.111739848163301</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5">
+      <c r="A163">
+        <v>4631</v>
+      </c>
+      <c r="B163">
+        <v>3.61</v>
+      </c>
+      <c r="C163">
+        <v>0.6000000000000001</v>
+      </c>
+      <c r="D163">
+        <v>-3.598794882638629</v>
+      </c>
+      <c r="E163">
+        <v>-0.1088623560627822</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5">
+      <c r="A164">
+        <v>4631</v>
+      </c>
+      <c r="B164">
+        <v>3.61</v>
+      </c>
+      <c r="C164">
+        <v>0.7000000000000001</v>
+      </c>
+      <c r="D164">
+        <v>-3.617390505648277</v>
+      </c>
+      <c r="E164">
+        <v>-0.09712722381701677</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5">
+      <c r="A165">
+        <v>4631</v>
+      </c>
+      <c r="B165">
+        <v>3.61</v>
+      </c>
+      <c r="C165">
+        <v>0.8</v>
+      </c>
+      <c r="D165">
+        <v>-3.62441792032533</v>
+      </c>
+      <c r="E165">
+        <v>-0.07382388323865574</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5">
+      <c r="A166">
+        <v>4631</v>
+      </c>
+      <c r="B166">
+        <v>3.61</v>
+      </c>
+      <c r="C166">
+        <v>0.9</v>
+      </c>
+      <c r="D166">
+        <v>-3.625914578422371</v>
+      </c>
+      <c r="E166">
+        <v>-0.04498978608028337</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5">
+      <c r="A167">
+        <v>4631</v>
+      </c>
+      <c r="B167">
+        <v>3.61</v>
+      </c>
+      <c r="C167">
+        <v>1</v>
+      </c>
+      <c r="D167">
+        <v>-3.611255547597501</v>
+      </c>
+      <c r="E167">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5">
+      <c r="A168">
+        <v>6083</v>
+      </c>
+      <c r="B168">
+        <v>3.971</v>
+      </c>
+      <c r="C168">
+        <v>0</v>
+      </c>
+      <c r="D168">
+        <v>-3.324181178750617</v>
+      </c>
+      <c r="E168">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5">
+      <c r="A169">
+        <v>6083</v>
+      </c>
+      <c r="B169">
+        <v>3.971</v>
+      </c>
+      <c r="C169">
+        <v>0.1</v>
+      </c>
+      <c r="D169">
+        <v>-3.396478241310193</v>
+      </c>
+      <c r="E169">
+        <v>-0.04181746435898237</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5">
+      <c r="A170">
+        <v>6083</v>
+      </c>
+      <c r="B170">
+        <v>3.971</v>
+      </c>
+      <c r="C170">
+        <v>0.2</v>
+      </c>
+      <c r="D170">
+        <v>-3.458241137795735</v>
+      </c>
+      <c r="E170">
+        <v>-0.07310076264393039</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5">
+      <c r="A171">
+        <v>6083</v>
+      </c>
+      <c r="B171">
+        <v>3.971</v>
+      </c>
+      <c r="C171">
+        <v>0.3</v>
+      </c>
+      <c r="D171">
+        <v>-3.509840730932367</v>
+      </c>
+      <c r="E171">
+        <v>-0.09422075757996806</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5">
+      <c r="A172">
+        <v>6083</v>
+      </c>
+      <c r="B172">
+        <v>3.971</v>
+      </c>
+      <c r="C172">
+        <v>0.4</v>
+      </c>
+      <c r="D172">
+        <v>-3.553330628974751</v>
+      </c>
+      <c r="E172">
+        <v>-0.107231057421759</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5">
+      <c r="A173">
+        <v>6083</v>
+      </c>
+      <c r="B173">
+        <v>3.971</v>
+      </c>
+      <c r="C173">
+        <v>0.5</v>
+      </c>
+      <c r="D173">
+        <v>-3.58803688303712</v>
+      </c>
+      <c r="E173">
+        <v>-0.1114577132835335</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5">
+      <c r="A174">
+        <v>6083</v>
+      </c>
+      <c r="B174">
+        <v>3.971</v>
+      </c>
+      <c r="C174">
+        <v>0.6000000000000001</v>
+      </c>
+      <c r="D174">
+        <v>-3.615062663740765</v>
+      </c>
+      <c r="E174">
+        <v>-0.1080038957865854</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5">
+      <c r="A175">
+        <v>6083</v>
+      </c>
+      <c r="B175">
+        <v>3.971</v>
+      </c>
+      <c r="C175">
+        <v>0.7000000000000001</v>
+      </c>
+      <c r="D175">
+        <v>-3.631835617047361</v>
+      </c>
+      <c r="E175">
+        <v>-0.094297250892587</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5">
+      <c r="A176">
+        <v>6083</v>
+      </c>
+      <c r="B176">
+        <v>3.971</v>
+      </c>
+      <c r="C176">
+        <v>0.8</v>
+      </c>
+      <c r="D176">
+        <v>-3.641225162337584</v>
+      </c>
+      <c r="E176">
+        <v>-0.07320719798221598</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5">
+      <c r="A177">
+        <v>6083</v>
+      </c>
+      <c r="B177">
+        <v>3.971</v>
+      </c>
+      <c r="C177">
+        <v>0.9</v>
+      </c>
+      <c r="D177">
+        <v>-3.642107052928966</v>
+      </c>
+      <c r="E177">
+        <v>-0.04360949037300421</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5">
+      <c r="A178">
+        <v>6083</v>
+      </c>
+      <c r="B178">
+        <v>3.971</v>
+      </c>
+      <c r="C178">
+        <v>1</v>
+      </c>
+      <c r="D178">
+        <v>-3.628977160756556</v>
+      </c>
+      <c r="E178">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5">
+      <c r="A179">
+        <v>7813</v>
+      </c>
+      <c r="B179">
+        <v>4.332</v>
+      </c>
+      <c r="C179">
+        <v>0</v>
+      </c>
+      <c r="D179">
+        <v>-3.336979244662767</v>
+      </c>
+      <c r="E179">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5">
+      <c r="A180">
+        <v>7813</v>
+      </c>
+      <c r="B180">
+        <v>4.332</v>
+      </c>
+      <c r="C180">
+        <v>0.1</v>
+      </c>
+      <c r="D180">
+        <v>-3.408451116542633</v>
+      </c>
+      <c r="E180">
+        <v>-0.04087492751618571</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5">
+      <c r="A181">
+        <v>7813</v>
+      </c>
+      <c r="B181">
+        <v>4.332</v>
+      </c>
+      <c r="C181">
+        <v>0.2</v>
+      </c>
+      <c r="D181">
+        <v>-3.469398272523909</v>
+      </c>
+      <c r="E181">
+        <v>-0.07122513913378148</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5">
+      <c r="A182">
+        <v>7813</v>
+      </c>
+      <c r="B182">
+        <v>4.332</v>
+      </c>
+      <c r="C182">
+        <v>0.3</v>
+      </c>
+      <c r="D182">
+        <v>-3.522265696919604</v>
+      </c>
+      <c r="E182">
+        <v>-0.09349561916579718</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5">
+      <c r="A183">
+        <v>7813</v>
+      </c>
+      <c r="B183">
+        <v>4.332</v>
+      </c>
+      <c r="C183">
+        <v>0.4</v>
+      </c>
+      <c r="D183">
+        <v>-3.566108172236689</v>
+      </c>
+      <c r="E183">
+        <v>-0.1067411501192024</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5">
+      <c r="A184">
+        <v>7813</v>
+      </c>
+      <c r="B184">
+        <v>4.332</v>
+      </c>
+      <c r="C184">
+        <v>0.5</v>
+      </c>
+      <c r="D184">
+        <v>-3.599977080214474</v>
+      </c>
+      <c r="E184">
+        <v>-0.1100131137333071</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5">
+      <c r="A185">
+        <v>7813</v>
+      </c>
+      <c r="B185">
+        <v>4.332</v>
+      </c>
+      <c r="C185">
+        <v>0.6000000000000001</v>
+      </c>
+      <c r="D185">
+        <v>-3.626486016514198</v>
+      </c>
+      <c r="E185">
+        <v>-0.1059251056693506</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5">
+      <c r="A186">
+        <v>7813</v>
+      </c>
+      <c r="B186">
+        <v>4.332</v>
+      </c>
+      <c r="C186">
+        <v>0.7000000000000001</v>
+      </c>
+      <c r="D186">
+        <v>-3.64504240695338</v>
+      </c>
+      <c r="E186">
+        <v>-0.09388455174485344</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5">
+      <c r="A187">
+        <v>7813</v>
+      </c>
+      <c r="B187">
+        <v>4.332</v>
+      </c>
+      <c r="C187">
+        <v>0.8</v>
+      </c>
+      <c r="D187">
+        <v>-3.653997728462638</v>
+      </c>
+      <c r="E187">
+        <v>-0.07224292889043071</v>
+      </c>
+    </row>
+    <row r="188" spans="1:5">
+      <c r="A188">
+        <v>7813</v>
+      </c>
+      <c r="B188">
+        <v>4.332</v>
+      </c>
+      <c r="C188">
+        <v>0.9</v>
+      </c>
+      <c r="D188">
+        <v>-3.655165113334387</v>
+      </c>
+      <c r="E188">
+        <v>-0.04281336939850056</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5">
+      <c r="A189">
+        <v>7813</v>
+      </c>
+      <c r="B189">
+        <v>4.332</v>
+      </c>
+      <c r="C189">
+        <v>1</v>
+      </c>
+      <c r="D189">
+        <v>-3.642948688299567</v>
+      </c>
+      <c r="E189">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
compleded CuAu fcc-cube sub5 calcs
</commit_message>
<xml_diff>
--- a/data/bimetallic_results/fcc-cube/fcc-cube_CuAu_data_sub5.xlsx
+++ b/data/bimetallic_results/fcc-cube/fcc-cube_CuAu_data_sub5.xlsx
@@ -386,7 +386,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E189"/>
+  <dimension ref="A1:E211"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -709,10 +709,10 @@
         <v>0.04761904761904762</v>
       </c>
       <c r="D19">
-        <v>-2.789574110896523</v>
+        <v>-2.789574110896522</v>
       </c>
       <c r="E19">
-        <v>-0.04987644809126657</v>
+        <v>-0.04987644809126612</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -729,7 +729,7 @@
         <v>-2.810169630509328</v>
       </c>
       <c r="E20">
-        <v>-0.06650193078835498</v>
+        <v>-0.06650193078835542</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -743,10 +743,10 @@
         <v>0.07936507936507936</v>
       </c>
       <c r="D21">
-        <v>-2.828241555670854</v>
+        <v>-2.829503352896493</v>
       </c>
       <c r="E21">
-        <v>-0.08060381903416447</v>
+        <v>-0.08186561625980415</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -760,10 +760,10 @@
         <v>0.09523809523809523</v>
       </c>
       <c r="D22">
-        <v>-2.850098872509298</v>
+        <v>-2.84757527805802</v>
       </c>
       <c r="E22">
-        <v>-0.09849109895689256</v>
+        <v>-0.09596750450561409</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -777,10 +777,10 @@
         <v>0.1111111111111111</v>
       </c>
       <c r="D23">
-        <v>-2.863006937906288</v>
+        <v>-2.864268735131928</v>
       </c>
       <c r="E23">
-        <v>-0.107429127438166</v>
+        <v>-0.1086909246638057</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -794,10 +794,10 @@
         <v>0.126984126984127</v>
       </c>
       <c r="D24">
-        <v>-2.882340660293454</v>
+        <v>-2.891289911734909</v>
       </c>
       <c r="E24">
-        <v>-0.1227928129096152</v>
+        <v>-0.1317420643510703</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -811,10 +811,10 @@
         <v>0.1428571428571428</v>
       </c>
       <c r="D25">
-        <v>-2.908100039670796</v>
+        <v>-2.904197977131899</v>
       </c>
       <c r="E25">
-        <v>-0.1445821553712405</v>
+        <v>-0.1406800928323437</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -828,10 +828,10 @@
         <v>0.1587301587301587</v>
       </c>
       <c r="D26">
-        <v>-2.921349138483738</v>
+        <v>-2.922269902293426</v>
       </c>
       <c r="E26">
-        <v>-0.1538612172684659</v>
+        <v>-0.1547819810781541</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -845,10 +845,10 @@
         <v>0.1746031746031746</v>
       </c>
       <c r="D27">
-        <v>-2.920945725379538</v>
+        <v>-2.938963359367334</v>
       </c>
       <c r="E27">
-        <v>-0.1494877672485502</v>
+        <v>-0.1675054012363462</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -862,10 +862,10 @@
         <v>0.1904761904761905</v>
       </c>
       <c r="D28">
-        <v>-2.954852723493532</v>
+        <v>-2.942938615547483</v>
       </c>
       <c r="E28">
-        <v>-0.1794247284468273</v>
+        <v>-0.1675106205007779</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -879,10 +879,10 @@
         <v>0.2063492063492063</v>
       </c>
       <c r="D29">
-        <v>-2.95176037625595</v>
+        <v>-2.969434516584886</v>
       </c>
       <c r="E29">
-        <v>-0.172362344293528</v>
+        <v>-0.1900364846224645</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -896,10 +896,10 @@
         <v>0.2222222222222222</v>
       </c>
       <c r="D30">
-        <v>-2.980556322501973</v>
+        <v>-2.994781965493504</v>
       </c>
       <c r="E30">
-        <v>-0.1971882536238345</v>
+        <v>-0.2114138966153662</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -913,10 +913,10 @@
         <v>0.2380952380952381</v>
       </c>
       <c r="D31">
-        <v>-2.999703272438241</v>
+        <v>-2.98812260757728</v>
       </c>
       <c r="E31">
-        <v>-0.2123651666443869</v>
+        <v>-0.2007845017834256</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -930,10 +930,10 @@
         <v>0.253968253968254</v>
       </c>
       <c r="D32">
-        <v>-2.994606284722475</v>
+        <v>-3.021677260138665</v>
       </c>
       <c r="E32">
-        <v>-0.2032981420129047</v>
+        <v>-0.2303691174290945</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -947,10 +947,10 @@
         <v>0.2698412698412698</v>
       </c>
       <c r="D33">
-        <v>-3.009527842491398</v>
+        <v>-2.998315777319972</v>
       </c>
       <c r="E33">
-        <v>-0.214249662866111</v>
+        <v>-0.203037597694685</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -964,10 +964,10 @@
         <v>0.2857142857142857</v>
       </c>
       <c r="D34">
-        <v>-3.028533220045101</v>
+        <v>-3.023951343248706</v>
       </c>
       <c r="E34">
-        <v>-0.229285003504097</v>
+        <v>-0.2247031267077024</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -981,10 +981,10 @@
         <v>0.3015873015873016</v>
       </c>
       <c r="D35">
-        <v>-3.019351713883343</v>
+        <v>-3.05285438299186</v>
       </c>
       <c r="E35">
-        <v>-0.2161334604266232</v>
+        <v>-0.2496361295351393</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -998,10 +998,10 @@
         <v>0.3174603174603174</v>
       </c>
       <c r="D36">
-        <v>-3.063362667386178</v>
+        <v>-3.096631396356998</v>
       </c>
       <c r="E36">
-        <v>-0.256174377013741</v>
+        <v>-0.2894431059845612</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -1015,10 +1015,10 @@
         <v>0.3333333333333333</v>
       </c>
       <c r="D37">
-        <v>-3.065829320437619</v>
+        <v>-3.025944818478751</v>
       </c>
       <c r="E37">
-        <v>-0.2546709931494662</v>
+        <v>-0.2147864911905981</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -1032,10 +1032,10 @@
         <v>0.3492063492063492</v>
       </c>
       <c r="D38">
-        <v>-3.037026970323365</v>
+        <v>-3.074847431246315</v>
       </c>
       <c r="E38">
-        <v>-0.221898606119495</v>
+        <v>-0.259719067042445</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -1049,10 +1049,10 @@
         <v>0.3650793650793651</v>
       </c>
       <c r="D39">
-        <v>-3.081098662663362</v>
+        <v>-3.112793932096346</v>
       </c>
       <c r="E39">
-        <v>-0.2620002615437762</v>
+        <v>-0.2936955309767604</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -1066,10 +1066,10 @@
         <v>0.3809523809523809</v>
       </c>
       <c r="D40">
-        <v>-3.092065937571363</v>
+        <v>-3.064014595074571</v>
       </c>
       <c r="E40">
-        <v>-0.2689974995360604</v>
+        <v>-0.2409461570392681</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -1083,10 +1083,10 @@
         <v>0.3968253968253968</v>
       </c>
       <c r="D41">
-        <v>-3.073656185118655</v>
+        <v>-3.064226025234246</v>
       </c>
       <c r="E41">
-        <v>-0.2466177101676352</v>
+        <v>-0.2371875502832268</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -1100,10 +1100,10 @@
         <v>0.4126984126984127</v>
       </c>
       <c r="D42">
-        <v>-3.098541898095871</v>
+        <v>-3.176089041568086</v>
       </c>
       <c r="E42">
-        <v>-0.2675333862291356</v>
+        <v>-0.3450805297013497</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -1117,10 +1117,10 @@
         <v>0.4285714285714285</v>
       </c>
       <c r="D43">
-        <v>-3.139479292821814</v>
+        <v>-3.104410243867193</v>
       </c>
       <c r="E43">
-        <v>-0.3045007440393612</v>
+        <v>-0.2694316950847409</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -1134,10 +1134,10 @@
         <v>0.4444444444444444</v>
       </c>
       <c r="D44">
-        <v>-3.153423368758159</v>
+        <v>-3.079474156405472</v>
       </c>
       <c r="E44">
-        <v>-0.3144747830599899</v>
+        <v>-0.2405255707073026</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -1151,10 +1151,10 @@
         <v>0.4603174603174603</v>
       </c>
       <c r="D45">
-        <v>-3.119471255952907</v>
+        <v>-3.162918684441564</v>
       </c>
       <c r="E45">
-        <v>-0.2765526333390218</v>
+        <v>-0.3200000618276784</v>
       </c>
     </row>
     <row r="46" spans="1:5">
@@ -1168,10 +1168,10 @@
         <v>0.4761904761904762</v>
       </c>
       <c r="D46">
-        <v>-3.118665382102996</v>
+        <v>-3.104881411711639</v>
       </c>
       <c r="E46">
-        <v>-0.271776722573394</v>
+        <v>-0.2579927521820373</v>
       </c>
     </row>
     <row r="47" spans="1:5">
@@ -1185,10 +1185,10 @@
         <v>0.492063492063492</v>
       </c>
       <c r="D47">
-        <v>-3.146574918671662</v>
+        <v>-3.179214459557329</v>
       </c>
       <c r="E47">
-        <v>-0.2957162222263434</v>
+        <v>-0.3283557631120104</v>
       </c>
     </row>
     <row r="48" spans="1:5">
@@ -1202,10 +1202,10 @@
         <v>0.5079365079365079</v>
       </c>
       <c r="D48">
-        <v>-3.155541111546033</v>
+        <v>-3.143812059801103</v>
       </c>
       <c r="E48">
-        <v>-0.3007123781849979</v>
+        <v>-0.2889833264400683</v>
       </c>
     </row>
     <row r="49" spans="1:5">
@@ -1219,10 +1219,10 @@
         <v>0.5238095238095238</v>
       </c>
       <c r="D49">
-        <v>-3.135438621456831</v>
+        <v>-3.104487213889615</v>
       </c>
       <c r="E49">
-        <v>-0.2766398511800796</v>
+        <v>-0.2456884436128632</v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -1236,10 +1236,10 @@
         <v>0.5396825396825397</v>
       </c>
       <c r="D50">
-        <v>-3.186242417610071</v>
+        <v>-3.145915384859503</v>
       </c>
       <c r="E50">
-        <v>-0.3234736104176026</v>
+        <v>-0.2831465776670345</v>
       </c>
     </row>
     <row r="51" spans="1:5">
@@ -1253,10 +1253,10 @@
         <v>0.5555555555555556</v>
       </c>
       <c r="D51">
-        <v>-3.189446388069909</v>
+        <v>-3.179452489377404</v>
       </c>
       <c r="E51">
-        <v>-0.3227075439617244</v>
+        <v>-0.3127136452692194</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -1270,10 +1270,10 @@
         <v>0.5714285714285714</v>
       </c>
       <c r="D52">
-        <v>-3.182553760843985</v>
+        <v>-3.167663414771268</v>
       </c>
       <c r="E52">
-        <v>-0.3118448798200841</v>
+        <v>-0.2969545337473667</v>
       </c>
     </row>
     <row r="53" spans="1:5">
@@ -1287,10 +1287,10 @@
         <v>0.5873015873015873</v>
       </c>
       <c r="D53">
-        <v>-3.175541855519404</v>
+        <v>-3.135942019610706</v>
       </c>
       <c r="E53">
-        <v>-0.3008629375797867</v>
+        <v>-0.2612631016710889</v>
       </c>
     </row>
     <row r="54" spans="1:5">
@@ -1304,10 +1304,10 @@
         <v>0.6031746031746031</v>
       </c>
       <c r="D54">
-        <v>-3.1905979654172</v>
+        <v>-3.191878665110361</v>
       </c>
       <c r="E54">
-        <v>-0.3119490105618659</v>
+        <v>-0.3132297102550265</v>
       </c>
     </row>
     <row r="55" spans="1:5">
@@ -1321,10 +1321,10 @@
         <v>0.6190476190476191</v>
       </c>
       <c r="D55">
-        <v>-3.133254836413261</v>
+        <v>-3.167780465434033</v>
       </c>
       <c r="E55">
-        <v>-0.2506358446422106</v>
+        <v>-0.2851614736629824</v>
       </c>
     </row>
     <row r="56" spans="1:5">
@@ -1338,10 +1338,10 @@
         <v>0.6349206349206349</v>
       </c>
       <c r="D56">
-        <v>-3.176800618940493</v>
+        <v>-3.165122152261961</v>
       </c>
       <c r="E56">
-        <v>-0.2902115902537257</v>
+        <v>-0.2785331235751944</v>
       </c>
     </row>
     <row r="57" spans="1:5">
@@ -1355,10 +1355,10 @@
         <v>0.6507936507936508</v>
       </c>
       <c r="D57">
-        <v>-3.176841089972586</v>
+        <v>-3.155910214509497</v>
       </c>
       <c r="E57">
-        <v>-0.2862820243701023</v>
+        <v>-0.2653511489070137</v>
       </c>
     </row>
     <row r="58" spans="1:5">
@@ -1372,10 +1372,10 @@
         <v>0.6666666666666666</v>
       </c>
       <c r="D58">
-        <v>-3.175976411261993</v>
+        <v>-3.156201431549261</v>
       </c>
       <c r="E58">
-        <v>-0.2814473087437932</v>
+        <v>-0.2616723290310614</v>
       </c>
     </row>
     <row r="59" spans="1:5">
@@ -1389,10 +1389,10 @@
         <v>0.6825396825396826</v>
       </c>
       <c r="D59">
-        <v>-3.145337328302018</v>
+        <v>-3.166251538741211</v>
       </c>
       <c r="E59">
-        <v>-0.2468381888681017</v>
+        <v>-0.2677523993072948</v>
       </c>
     </row>
     <row r="60" spans="1:5">
@@ -1406,10 +1406,10 @@
         <v>0.6984126984126984</v>
       </c>
       <c r="D60">
-        <v>-3.163976783395619</v>
+        <v>-3.160768988150287</v>
       </c>
       <c r="E60">
-        <v>-0.2615076070459857</v>
+        <v>-0.2582998118006542</v>
       </c>
     </row>
     <row r="61" spans="1:5">
@@ -1423,10 +1423,10 @@
         <v>0.7142857142857143</v>
       </c>
       <c r="D61">
-        <v>-3.139624402834649</v>
+        <v>-3.152971211181676</v>
       </c>
       <c r="E61">
-        <v>-0.2331851895692995</v>
+        <v>-0.2465319979163264</v>
       </c>
     </row>
     <row r="62" spans="1:5">
@@ -1440,10 +1440,10 @@
         <v>0.7301587301587301</v>
       </c>
       <c r="D62">
-        <v>-3.14761803753259</v>
+        <v>-3.130545926172879</v>
       </c>
       <c r="E62">
-        <v>-0.2372087873515235</v>
+        <v>-0.220136675991813</v>
       </c>
     </row>
     <row r="63" spans="1:5">
@@ -1457,10 +1457,10 @@
         <v>0.746031746031746</v>
       </c>
       <c r="D63">
-        <v>-3.139574087555343</v>
+        <v>-3.142006109999828</v>
       </c>
       <c r="E63">
-        <v>-0.2251948004585606</v>
+        <v>-0.2276268229030453</v>
       </c>
     </row>
     <row r="64" spans="1:5">
@@ -1474,10 +1474,10 @@
         <v>0.7619047619047619</v>
       </c>
       <c r="D64">
-        <v>-3.136523559408903</v>
+        <v>-3.133574029197066</v>
       </c>
       <c r="E64">
-        <v>-0.2181742353964038</v>
+        <v>-0.2152247051845666</v>
       </c>
     </row>
     <row r="65" spans="1:5">
@@ -1491,10 +1491,10 @@
         <v>0.7777777777777778</v>
       </c>
       <c r="D65">
-        <v>-3.129372178299302</v>
+        <v>-3.129501555241141</v>
       </c>
       <c r="E65">
-        <v>-0.2070528173710866</v>
+        <v>-0.2071821943129251</v>
       </c>
     </row>
     <row r="66" spans="1:5">
@@ -1508,10 +1508,10 @@
         <v>0.7936507936507936</v>
       </c>
       <c r="D66">
-        <v>-3.125170327401539</v>
+        <v>-3.122738304957056</v>
       </c>
       <c r="E66">
-        <v>-0.1988809295576067</v>
+        <v>-0.1964489071131238</v>
       </c>
     </row>
     <row r="67" spans="1:5">
@@ -1525,10 +1525,10 @@
         <v>0.8095238095238095</v>
       </c>
       <c r="D67">
-        <v>-3.118407077117454</v>
+        <v>-3.11378920523712</v>
       </c>
       <c r="E67">
-        <v>-0.1881476423578049</v>
+        <v>-0.1835297704774715</v>
       </c>
     </row>
     <row r="68" spans="1:5">
@@ -1542,10 +1542,10 @@
         <v>0.8253968253968254</v>
       </c>
       <c r="D68">
-        <v>-3.107025954953037</v>
+        <v>-3.105615878318036</v>
       </c>
       <c r="E68">
-        <v>-0.1727964832776717</v>
+        <v>-0.1713864066426712</v>
       </c>
     </row>
     <row r="69" spans="1:5">
@@ -1559,10 +1559,10 @@
         <v>0.8412698412698413</v>
       </c>
       <c r="D69">
-        <v>-3.104492445723768</v>
+        <v>-3.095644832788619</v>
       </c>
       <c r="E69">
-        <v>-0.1662929371326861</v>
+        <v>-0.157445324197537</v>
       </c>
     </row>
     <row r="70" spans="1:5">
@@ -1576,10 +1576,10 @@
         <v>0.8571428571428571</v>
       </c>
       <c r="D70">
-        <v>-3.089903528314018</v>
+        <v>-3.093240700501187</v>
       </c>
       <c r="E70">
-        <v>-0.1477339828072196</v>
+        <v>-0.1510711549943891</v>
       </c>
     </row>
     <row r="71" spans="1:5">
@@ -1593,10 +1593,10 @@
         <v>0.873015873015873</v>
       </c>
       <c r="D71">
-        <v>-3.083010901088095</v>
+        <v>-3.086218696333426</v>
       </c>
       <c r="E71">
-        <v>-0.1368713186655797</v>
+        <v>-0.1400791139109113</v>
       </c>
     </row>
     <row r="72" spans="1:5">
@@ -1610,10 +1610,10 @@
         <v>0.8888888888888888</v>
       </c>
       <c r="D72">
-        <v>-3.070478456172355</v>
+        <v>-3.073686251417686</v>
       </c>
       <c r="E72">
-        <v>-0.1203688368341242</v>
+        <v>-0.1235766320794544</v>
       </c>
     </row>
     <row r="73" spans="1:5">
@@ -1627,10 +1627,10 @@
         <v>0.9047619047619048</v>
       </c>
       <c r="D73">
-        <v>-3.057946011256613</v>
+        <v>-3.06230512925327</v>
       </c>
       <c r="E73">
-        <v>-0.1038663550026654</v>
+        <v>-0.1082254729993219</v>
       </c>
     </row>
     <row r="74" spans="1:5">
@@ -1644,10 +1644,10 @@
         <v>0.9206349206349206</v>
       </c>
       <c r="D74">
-        <v>-3.048621361586205</v>
+        <v>-3.049772684337528</v>
       </c>
       <c r="E74">
-        <v>-0.09057166841654107</v>
+        <v>-0.0917229911678642</v>
       </c>
     </row>
     <row r="75" spans="1:5">
@@ -1664,7 +1664,7 @@
         <v>-3.037240239421788</v>
       </c>
       <c r="E75">
-        <v>-0.0752205093364077</v>
+        <v>-0.07522050933640725</v>
       </c>
     </row>
     <row r="76" spans="1:5">
@@ -1763,10 +1763,10 @@
         <v>0.1</v>
       </c>
       <c r="D81">
-        <v>-3.058356608783145</v>
+        <v>-3.052352164398814</v>
       </c>
       <c r="E81">
-        <v>-0.07133700030342593</v>
+        <v>-0.06533255591909493</v>
       </c>
     </row>
     <row r="82" spans="1:5">
@@ -1780,10 +1780,10 @@
         <v>0.2</v>
       </c>
       <c r="D82">
-        <v>-3.135725781470565</v>
+        <v>-3.128901728878322</v>
       </c>
       <c r="E82">
-        <v>-0.1215668693362884</v>
+        <v>-0.114742816744045</v>
       </c>
     </row>
     <row r="83" spans="1:5">
@@ -1797,10 +1797,10 @@
         <v>0.3</v>
       </c>
       <c r="D83">
-        <v>-3.192583078351433</v>
+        <v>-3.203835278700523</v>
       </c>
       <c r="E83">
-        <v>-0.1512848625625987</v>
+        <v>-0.1625370629116882</v>
       </c>
     </row>
     <row r="84" spans="1:5">
@@ -1814,10 +1814,10 @@
         <v>0.4</v>
       </c>
       <c r="D84">
-        <v>-3.254713279152627</v>
+        <v>-3.243213570831897</v>
       </c>
       <c r="E84">
-        <v>-0.186275759709235</v>
+        <v>-0.1747760513885053</v>
       </c>
     </row>
     <row r="85" spans="1:5">
@@ -1831,10 +1831,10 @@
         <v>0.5</v>
       </c>
       <c r="D85">
-        <v>-3.306201424589144</v>
+        <v>-3.303406177687894</v>
       </c>
       <c r="E85">
-        <v>-0.2106246014911946</v>
+        <v>-0.2078293545899441</v>
       </c>
     </row>
     <row r="86" spans="1:5">
@@ -1848,10 +1848,10 @@
         <v>0.6000000000000001</v>
       </c>
       <c r="D86">
-        <v>-3.320452310899221</v>
+        <v>-3.330109806467956</v>
       </c>
       <c r="E86">
-        <v>-0.1977361841467136</v>
+        <v>-0.2073936797154492</v>
       </c>
     </row>
     <row r="87" spans="1:5">
@@ -1865,10 +1865,10 @@
         <v>0.7000000000000001</v>
       </c>
       <c r="D87">
-        <v>-3.329520207746302</v>
+        <v>-3.34549140488265</v>
       </c>
       <c r="E87">
-        <v>-0.1796647773392374</v>
+        <v>-0.1956359744755855</v>
       </c>
     </row>
     <row r="88" spans="1:5">
@@ -1882,10 +1882,10 @@
         <v>0.8</v>
       </c>
       <c r="D88">
-        <v>-3.35077729546683</v>
+        <v>-3.358235331225703</v>
       </c>
       <c r="E88">
-        <v>-0.1737825614052075</v>
+        <v>-0.1812405971640809</v>
       </c>
     </row>
     <row r="89" spans="1:5">
@@ -1899,10 +1899,10 @@
         <v>0.9</v>
       </c>
       <c r="D89">
-        <v>-3.318157016472849</v>
+        <v>-3.318300358590588</v>
       </c>
       <c r="E89">
-        <v>-0.1140229787566692</v>
+        <v>-0.1141663208744083</v>
       </c>
     </row>
     <row r="90" spans="1:5">
@@ -1950,10 +1950,10 @@
         <v>0.1</v>
       </c>
       <c r="D92">
-        <v>-3.161581195732908</v>
+        <v>-3.165560653984654</v>
       </c>
       <c r="E92">
-        <v>-0.06692632511325503</v>
+        <v>-0.07090578336500153</v>
       </c>
     </row>
     <row r="93" spans="1:5">
@@ -1967,10 +1967,10 @@
         <v>0.2</v>
       </c>
       <c r="D93">
-        <v>-3.236372728691916</v>
+        <v>-3.230675911184664</v>
       </c>
       <c r="E93">
-        <v>-0.1136006076861698</v>
+        <v>-0.1079037901789186</v>
       </c>
     </row>
     <row r="94" spans="1:5">
@@ -1984,10 +1984,10 @@
         <v>0.3</v>
       </c>
       <c r="D94">
-        <v>-3.288338270252288</v>
+        <v>-3.293745178898482</v>
       </c>
       <c r="E94">
-        <v>-0.1374488988604488</v>
+        <v>-0.1428558075066433</v>
       </c>
     </row>
     <row r="95" spans="1:5">
@@ -2001,10 +2001,10 @@
         <v>0.4</v>
       </c>
       <c r="D95">
-        <v>-3.354550452239324</v>
+        <v>-3.338102298563276</v>
       </c>
       <c r="E95">
-        <v>-0.1755438304613919</v>
+        <v>-0.1590956767853433</v>
       </c>
     </row>
     <row r="96" spans="1:5">
@@ -2018,10 +2018,10 @@
         <v>0.5</v>
       </c>
       <c r="D96">
-        <v>-3.384297884273012</v>
+        <v>-3.383120087957724</v>
       </c>
       <c r="E96">
-        <v>-0.1771740121089866</v>
+        <v>-0.1759962157936981</v>
       </c>
     </row>
     <row r="97" spans="1:5">
@@ -2035,10 +2035,10 @@
         <v>0.6000000000000001</v>
       </c>
       <c r="D97">
-        <v>-3.407656001362706</v>
+        <v>-3.413406206242885</v>
       </c>
       <c r="E97">
-        <v>-0.172414878812587</v>
+        <v>-0.178165083692766</v>
       </c>
     </row>
     <row r="98" spans="1:5">
@@ -2052,10 +2052,10 @@
         <v>0.7000000000000001</v>
       </c>
       <c r="D98">
-        <v>-3.425750486464414</v>
+        <v>-3.429671939737385</v>
       </c>
       <c r="E98">
-        <v>-0.1623921135282019</v>
+        <v>-0.1663135668011723</v>
       </c>
     </row>
     <row r="99" spans="1:5">
@@ -2069,10 +2069,10 @@
         <v>0.8</v>
       </c>
       <c r="D99">
-        <v>-3.424499944765616</v>
+        <v>-3.426313838489969</v>
       </c>
       <c r="E99">
-        <v>-0.1330243214433109</v>
+        <v>-0.1348382151676639</v>
       </c>
     </row>
     <row r="100" spans="1:5">
@@ -2086,10 +2086,10 @@
         <v>0.9</v>
       </c>
       <c r="D100">
-        <v>-3.413115677387186</v>
+        <v>-3.408337465773274</v>
       </c>
       <c r="E100">
-        <v>-0.09352280367878718</v>
+        <v>-0.08874459206487462</v>
       </c>
     </row>
     <row r="101" spans="1:5">
@@ -2137,10 +2137,10 @@
         <v>0.1</v>
       </c>
       <c r="D103">
-        <v>-3.233096084150288</v>
+        <v>-3.233775149092084</v>
       </c>
       <c r="E103">
-        <v>-0.05699878583446827</v>
+        <v>-0.05767785077626408</v>
       </c>
     </row>
     <row r="104" spans="1:5">
@@ -2154,10 +2154,10 @@
         <v>0.2</v>
       </c>
       <c r="D104">
-        <v>-3.304764538410597</v>
+        <v>-3.302289546133792</v>
       </c>
       <c r="E104">
-        <v>-0.0998100244371698</v>
+        <v>-0.09733503216036565</v>
       </c>
     </row>
     <row r="105" spans="1:5">
@@ -2171,10 +2171,10 @@
         <v>0.3</v>
       </c>
       <c r="D105">
-        <v>-3.360443864832046</v>
+        <v>-3.359619751918806</v>
       </c>
       <c r="E105">
-        <v>-0.1266321352010125</v>
+        <v>-0.1258080222877731</v>
       </c>
     </row>
     <row r="106" spans="1:5">
@@ -2188,10 +2188,10 @@
         <v>0.4</v>
       </c>
       <c r="D106">
-        <v>-3.403472159370311</v>
+        <v>-3.403808194731244</v>
       </c>
       <c r="E106">
-        <v>-0.1408032140816711</v>
+        <v>-0.1411392494426043</v>
       </c>
     </row>
     <row r="107" spans="1:5">
@@ -2205,10 +2205,10 @@
         <v>0.5</v>
       </c>
       <c r="D107">
-        <v>-3.441249060163437</v>
+        <v>-3.433047390979762</v>
       </c>
       <c r="E107">
-        <v>-0.1497228992171906</v>
+        <v>-0.1415212300335154</v>
       </c>
     </row>
     <row r="108" spans="1:5">
@@ -2222,10 +2222,10 @@
         <v>0.6000000000000001</v>
       </c>
       <c r="D108">
-        <v>-3.464903714971963</v>
+        <v>-3.463408641886657</v>
       </c>
       <c r="E108">
-        <v>-0.1445203383681097</v>
+        <v>-0.1430252652828041</v>
       </c>
     </row>
     <row r="109" spans="1:5">
@@ -2239,10 +2239,10 @@
         <v>0.7000000000000001</v>
       </c>
       <c r="D109">
-        <v>-3.476534904753164</v>
+        <v>-3.479598645440032</v>
       </c>
       <c r="E109">
-        <v>-0.1272943124917048</v>
+        <v>-0.1303580531785731</v>
       </c>
     </row>
     <row r="110" spans="1:5">
@@ -2256,10 +2256,10 @@
         <v>0.8</v>
       </c>
       <c r="D110">
-        <v>-3.487543401036584</v>
+        <v>-3.487589356753714</v>
       </c>
       <c r="E110">
-        <v>-0.1094455931175183</v>
+        <v>-0.1094915488346483</v>
       </c>
     </row>
     <row r="111" spans="1:5">
@@ -2273,10 +2273,10 @@
         <v>0.9</v>
       </c>
       <c r="D111">
-        <v>-3.477519463532454</v>
+        <v>-3.476295361095636</v>
       </c>
       <c r="E111">
-        <v>-0.07056443995578171</v>
+        <v>-0.0693403375189639</v>
       </c>
     </row>
     <row r="112" spans="1:5">
@@ -2324,10 +2324,10 @@
         <v>0.1</v>
       </c>
       <c r="D114">
-        <v>-3.279642334612179</v>
+        <v>-3.276458331473056</v>
       </c>
       <c r="E114">
-        <v>-0.05386342279105838</v>
+        <v>-0.05067941965193512</v>
       </c>
     </row>
     <row r="115" spans="1:5">
@@ -2341,10 +2341,10 @@
         <v>0.2</v>
       </c>
       <c r="D115">
-        <v>-3.344053583592614</v>
+        <v>-3.341346007467622</v>
       </c>
       <c r="E115">
-        <v>-0.08896606155619136</v>
+        <v>-0.08625848543119918</v>
       </c>
     </row>
     <row r="116" spans="1:5">
@@ -2358,10 +2358,10 @@
         <v>0.3</v>
       </c>
       <c r="D116">
-        <v>-3.394086560507519</v>
+        <v>-3.39930632585253</v>
       </c>
       <c r="E116">
-        <v>-0.1096904282557944</v>
+        <v>-0.1149101936008061</v>
       </c>
     </row>
     <row r="117" spans="1:5">
@@ -2375,10 +2375,10 @@
         <v>0.4</v>
       </c>
       <c r="D117">
-        <v>-3.444413412094474</v>
+        <v>-3.441631472681903</v>
       </c>
       <c r="E117">
-        <v>-0.1307086696274469</v>
+        <v>-0.1279267302148763</v>
       </c>
     </row>
     <row r="118" spans="1:5">
@@ -2392,10 +2392,10 @@
         <v>0.5</v>
       </c>
       <c r="D118">
-        <v>-3.480654289073926</v>
+        <v>-3.479570543702916</v>
       </c>
       <c r="E118">
-        <v>-0.1376409363915967</v>
+        <v>-0.1365571910205874</v>
       </c>
     </row>
     <row r="119" spans="1:5">
@@ -2409,10 +2409,10 @@
         <v>0.6000000000000001</v>
       </c>
       <c r="D119">
-        <v>-3.500354909432203</v>
+        <v>-3.503338692334431</v>
       </c>
       <c r="E119">
-        <v>-0.1280329465345722</v>
+        <v>-0.1310167294368001</v>
       </c>
     </row>
     <row r="120" spans="1:5">
@@ -2426,10 +2426,10 @@
         <v>0.7000000000000001</v>
       </c>
       <c r="D120">
-        <v>-3.515197055561998</v>
+        <v>-3.519260550058773</v>
       </c>
       <c r="E120">
-        <v>-0.1135664824490653</v>
+        <v>-0.1176299769458403</v>
       </c>
     </row>
     <row r="121" spans="1:5">
@@ -2443,10 +2443,10 @@
         <v>0.8</v>
       </c>
       <c r="D121">
-        <v>-3.522287844998943</v>
+        <v>-3.523658164389187</v>
       </c>
       <c r="E121">
-        <v>-0.09134866167070799</v>
+        <v>-0.09271898106095167</v>
       </c>
     </row>
     <row r="122" spans="1:5">
@@ -2460,10 +2460,10 @@
         <v>0.9</v>
       </c>
       <c r="D122">
-        <v>-3.521505561845264</v>
+        <v>-3.521711542155269</v>
       </c>
       <c r="E122">
-        <v>-0.06125776830172747</v>
+        <v>-0.06146374861173198</v>
       </c>
     </row>
     <row r="123" spans="1:5">
@@ -2511,10 +2511,10 @@
         <v>0.1</v>
       </c>
       <c r="D125">
-        <v>-3.314745822582975</v>
+        <v>-3.316380124248854</v>
       </c>
       <c r="E125">
-        <v>-0.04799991524422165</v>
+        <v>-0.04963421691010117</v>
       </c>
     </row>
     <row r="126" spans="1:5">
@@ -2528,10 +2528,10 @@
         <v>0.2</v>
       </c>
       <c r="D126">
-        <v>-3.377927488883896</v>
+        <v>-3.379969259274899</v>
       </c>
       <c r="E126">
-        <v>-0.08150075558407144</v>
+        <v>-0.08354252597507417</v>
       </c>
     </row>
     <row r="127" spans="1:5">
@@ -2545,10 +2545,10 @@
         <v>0.3</v>
       </c>
       <c r="D127">
-        <v>-3.431028964847889</v>
+        <v>-3.43257288623901</v>
       </c>
       <c r="E127">
-        <v>-0.1049214055869938</v>
+        <v>-0.1064653269781153</v>
       </c>
     </row>
     <row r="128" spans="1:5">
@@ -2562,10 +2562,10 @@
         <v>0.4</v>
       </c>
       <c r="D128">
-        <v>-3.475518749631872</v>
+        <v>-3.475545023111857</v>
       </c>
       <c r="E128">
-        <v>-0.1197303644099061</v>
+        <v>-0.1197566378898915</v>
       </c>
     </row>
     <row r="129" spans="1:5">
@@ -2579,10 +2579,10 @@
         <v>0.5</v>
       </c>
       <c r="D129">
-        <v>-3.506959582804033</v>
+        <v>-3.511702278781871</v>
       </c>
       <c r="E129">
-        <v>-0.1214903716209965</v>
+        <v>-0.1262330675988343</v>
       </c>
     </row>
     <row r="130" spans="1:5">
@@ -2596,10 +2596,10 @@
         <v>0.6000000000000001</v>
       </c>
       <c r="D130">
-        <v>-3.535781107116629</v>
+        <v>-3.533902133859949</v>
       </c>
       <c r="E130">
-        <v>-0.1206310699725217</v>
+        <v>-0.1187520967158415</v>
       </c>
     </row>
     <row r="131" spans="1:5">
@@ -2613,10 +2613,10 @@
         <v>0.7000000000000001</v>
       </c>
       <c r="D131">
-        <v>-3.553393583412525</v>
+        <v>-3.550919440324825</v>
       </c>
       <c r="E131">
-        <v>-0.1085627203073463</v>
+        <v>-0.1060885772196465</v>
       </c>
     </row>
     <row r="132" spans="1:5">
@@ -2630,10 +2630,10 @@
         <v>0.8</v>
       </c>
       <c r="D132">
-        <v>-3.562021687351217</v>
+        <v>-3.55788704124627</v>
       </c>
       <c r="E132">
-        <v>-0.08750999828496775</v>
+        <v>-0.08337535218002123</v>
       </c>
     </row>
     <row r="133" spans="1:5">
@@ -2647,10 +2647,10 @@
         <v>0.9</v>
       </c>
       <c r="D133">
-        <v>-3.56071317867139</v>
+        <v>-3.559574622101302</v>
       </c>
       <c r="E133">
-        <v>-0.05652066364407043</v>
+        <v>-0.05538210707398167</v>
       </c>
     </row>
     <row r="134" spans="1:5">
@@ -2698,10 +2698,10 @@
         <v>0.1</v>
       </c>
       <c r="D136">
-        <v>-3.342018340796063</v>
+        <v>-3.342055462953265</v>
       </c>
       <c r="E136">
-        <v>-0.04678174642197153</v>
+        <v>-0.04681886857917394</v>
       </c>
     </row>
     <row r="137" spans="1:5">
@@ -2715,10 +2715,10 @@
         <v>0.2</v>
       </c>
       <c r="D137">
-        <v>-3.40215548275237</v>
+        <v>-3.402529623821039</v>
       </c>
       <c r="E137">
-        <v>-0.0769792032504899</v>
+        <v>-0.07735334431915941</v>
       </c>
     </row>
     <row r="138" spans="1:5">
@@ -2732,10 +2732,10 @@
         <v>0.3</v>
       </c>
       <c r="D138">
-        <v>-3.456100152157441</v>
+        <v>-3.45675534551541</v>
       </c>
       <c r="E138">
-        <v>-0.1009841875277733</v>
+        <v>-0.1016393808857421</v>
       </c>
     </row>
     <row r="139" spans="1:5">
@@ -2749,10 +2749,10 @@
         <v>0.4</v>
       </c>
       <c r="D139">
-        <v>-3.499380358962707</v>
+        <v>-3.499731813798032</v>
       </c>
       <c r="E139">
-        <v>-0.1143247092052506</v>
+        <v>-0.1146761640405758</v>
       </c>
     </row>
     <row r="140" spans="1:5">
@@ -2766,10 +2766,10 @@
         <v>0.5</v>
       </c>
       <c r="D140">
-        <v>-3.534958005770232</v>
+        <v>-3.535107894336885</v>
       </c>
       <c r="E140">
-        <v>-0.119962670884987</v>
+        <v>-0.1201125594516406</v>
       </c>
     </row>
     <row r="141" spans="1:5">
@@ -2783,10 +2783,10 @@
         <v>0.6000000000000001</v>
       </c>
       <c r="D141">
-        <v>-3.559010414775953</v>
+        <v>-3.559273514341921</v>
       </c>
       <c r="E141">
-        <v>-0.1140753947629201</v>
+        <v>-0.1143384943288874</v>
       </c>
     </row>
     <row r="142" spans="1:5">
@@ -2800,10 +2800,10 @@
         <v>0.7000000000000001</v>
       </c>
       <c r="D142">
-        <v>-3.578640233582048</v>
+        <v>-3.574932443649902</v>
       </c>
       <c r="E142">
-        <v>-0.1037655284412266</v>
+        <v>-0.1000577385090803</v>
       </c>
     </row>
     <row r="143" spans="1:5">
@@ -2817,10 +2817,10 @@
         <v>0.8</v>
       </c>
       <c r="D143">
-        <v>-3.585101801018822</v>
+        <v>-3.587107211351</v>
       </c>
       <c r="E143">
-        <v>-0.08028741075021195</v>
+        <v>-0.08229282108239</v>
       </c>
     </row>
     <row r="144" spans="1:5">
@@ -2834,10 +2834,10 @@
         <v>0.9</v>
       </c>
       <c r="D144">
-        <v>-3.58303208388604</v>
+        <v>-3.586411380511542</v>
       </c>
       <c r="E144">
-        <v>-0.04827800848964131</v>
+        <v>-0.05165730511514394</v>
       </c>
     </row>
     <row r="145" spans="1:5">
@@ -2885,10 +2885,10 @@
         <v>0.1</v>
       </c>
       <c r="D147">
-        <v>-3.364323948766299</v>
+        <v>-3.363745871259663</v>
       </c>
       <c r="E147">
-        <v>-0.04449563731934081</v>
+        <v>-0.04391755981270506</v>
       </c>
     </row>
     <row r="148" spans="1:5">
@@ -2902,10 +2902,10 @@
         <v>0.2</v>
       </c>
       <c r="D148">
-        <v>-3.424525887254642</v>
+        <v>-3.425400546066034</v>
       </c>
       <c r="E148">
-        <v>-0.07453445656681357</v>
+        <v>-0.07540911537820572</v>
       </c>
     </row>
     <row r="149" spans="1:5">
@@ -2919,10 +2919,10 @@
         <v>0.3</v>
       </c>
       <c r="D149">
-        <v>-3.477855097229322</v>
+        <v>-3.477116442472978</v>
       </c>
       <c r="E149">
-        <v>-0.09770054730062272</v>
+        <v>-0.09696189254427923</v>
       </c>
     </row>
     <row r="150" spans="1:5">
@@ -2936,10 +2936,10 @@
         <v>0.4</v>
       </c>
       <c r="D150">
-        <v>-3.522939214065749</v>
+        <v>-3.520626620067804</v>
       </c>
       <c r="E150">
-        <v>-0.1126215448961794</v>
+        <v>-0.1103089508982344</v>
       </c>
     </row>
     <row r="151" spans="1:5">
@@ -2953,10 +2953,10 @@
         <v>0.5</v>
       </c>
       <c r="D151">
-        <v>-3.556009560925981</v>
+        <v>-3.556595026310356</v>
       </c>
       <c r="E151">
-        <v>-0.1155287725155412</v>
+        <v>-0.1161142378999163</v>
       </c>
     </row>
     <row r="152" spans="1:5">
@@ -2970,10 +2970,10 @@
         <v>0.6000000000000001</v>
       </c>
       <c r="D152">
-        <v>-3.58246111752868</v>
+        <v>-3.584440334055028</v>
       </c>
       <c r="E152">
-        <v>-0.1118172098773693</v>
+        <v>-0.1137964264037177</v>
       </c>
     </row>
     <row r="153" spans="1:5">
@@ -2987,10 +2987,10 @@
         <v>0.7000000000000001</v>
       </c>
       <c r="D153">
-        <v>-3.600001081311948</v>
+        <v>-3.599596624724711</v>
       </c>
       <c r="E153">
-        <v>-0.09919405441976648</v>
+        <v>-0.0987895978325295</v>
       </c>
     </row>
     <row r="154" spans="1:5">
@@ -3004,10 +3004,10 @@
         <v>0.8</v>
       </c>
       <c r="D154">
-        <v>-3.608271653611407</v>
+        <v>-3.608383923088095</v>
       </c>
       <c r="E154">
-        <v>-0.07730150747835596</v>
+        <v>-0.07741377695504326</v>
       </c>
     </row>
     <row r="155" spans="1:5">
@@ -3021,10 +3021,10 @@
         <v>0.9</v>
       </c>
       <c r="D155">
-        <v>-3.610087355988972</v>
+        <v>-3.607447900003985</v>
       </c>
       <c r="E155">
-        <v>-0.04895409061504935</v>
+        <v>-0.04631463463006286</v>
       </c>
     </row>
     <row r="156" spans="1:5">
@@ -3072,10 +3072,10 @@
         <v>0.1</v>
       </c>
       <c r="D158">
-        <v>-3.381484449756316</v>
+        <v>-3.381550268566277</v>
       </c>
       <c r="E158">
-        <v>-0.04320569945753716</v>
+        <v>-0.04327151826749853</v>
       </c>
     </row>
     <row r="159" spans="1:5">
@@ -3089,10 +3089,10 @@
         <v>0.2</v>
       </c>
       <c r="D159">
-        <v>-3.442508782265875</v>
+        <v>-3.443096931119976</v>
       </c>
       <c r="E159">
-        <v>-0.07389927671168239</v>
+        <v>-0.07448742556578303</v>
       </c>
     </row>
     <row r="160" spans="1:5">
@@ -3106,10 +3106,10 @@
         <v>0.3</v>
       </c>
       <c r="D160">
-        <v>-3.493856201376004</v>
+        <v>-3.496281691272348</v>
       </c>
       <c r="E160">
-        <v>-0.09491594056639796</v>
+        <v>-0.09734143046274157</v>
       </c>
     </row>
     <row r="161" spans="1:5">
@@ -3123,10 +3123,10 @@
         <v>0.4</v>
       </c>
       <c r="D161">
-        <v>-3.536289868406675</v>
+        <v>-3.537710678123374</v>
       </c>
       <c r="E161">
-        <v>-0.1070188523416555</v>
+        <v>-0.108439662058355</v>
       </c>
     </row>
     <row r="162" spans="1:5">
@@ -3140,10 +3140,10 @@
         <v>0.5</v>
       </c>
       <c r="D162">
-        <v>-3.571341619483734</v>
+        <v>-3.572872326656683</v>
       </c>
       <c r="E162">
-        <v>-0.111739848163301</v>
+        <v>-0.1132705553362503</v>
       </c>
     </row>
     <row r="163" spans="1:5">
@@ -3157,10 +3157,10 @@
         <v>0.6000000000000001</v>
       </c>
       <c r="D163">
-        <v>-3.598794882638629</v>
+        <v>-3.598795191384115</v>
       </c>
       <c r="E163">
-        <v>-0.1088623560627822</v>
+        <v>-0.1088626648082687</v>
       </c>
     </row>
     <row r="164" spans="1:5">
@@ -3174,10 +3174,10 @@
         <v>0.7000000000000001</v>
       </c>
       <c r="D164">
-        <v>-3.617390505648277</v>
+        <v>-3.616337891114114</v>
       </c>
       <c r="E164">
-        <v>-0.09712722381701677</v>
+        <v>-0.09607460928285405</v>
       </c>
     </row>
     <row r="165" spans="1:5">
@@ -3191,10 +3191,10 @@
         <v>0.8</v>
       </c>
       <c r="D165">
-        <v>-3.62441792032533</v>
+        <v>-3.625927741632625</v>
       </c>
       <c r="E165">
-        <v>-0.07382388323865574</v>
+        <v>-0.07533370454595167</v>
       </c>
     </row>
     <row r="166" spans="1:5">
@@ -3208,10 +3208,10 @@
         <v>0.9</v>
       </c>
       <c r="D166">
-        <v>-3.625914578422371</v>
+        <v>-3.62558981948986</v>
       </c>
       <c r="E166">
-        <v>-0.04498978608028337</v>
+        <v>-0.04466502714777276</v>
       </c>
     </row>
     <row r="167" spans="1:5">
@@ -3259,10 +3259,10 @@
         <v>0.1</v>
       </c>
       <c r="D169">
-        <v>-3.396478241310193</v>
+        <v>-3.396237803348463</v>
       </c>
       <c r="E169">
-        <v>-0.04181746435898237</v>
+        <v>-0.04157702639725214</v>
       </c>
     </row>
     <row r="170" spans="1:5">
@@ -3276,10 +3276,10 @@
         <v>0.2</v>
       </c>
       <c r="D170">
-        <v>-3.458241137795735</v>
+        <v>-3.457367280401124</v>
       </c>
       <c r="E170">
-        <v>-0.07310076264393039</v>
+        <v>-0.07222690524931963</v>
       </c>
     </row>
     <row r="171" spans="1:5">
@@ -3293,10 +3293,10 @@
         <v>0.3</v>
       </c>
       <c r="D171">
-        <v>-3.509840730932367</v>
+        <v>-3.509102805974914</v>
       </c>
       <c r="E171">
-        <v>-0.09422075757996806</v>
+        <v>-0.09348283262251522</v>
       </c>
     </row>
     <row r="172" spans="1:5">
@@ -3310,10 +3310,10 @@
         <v>0.4</v>
       </c>
       <c r="D172">
-        <v>-3.553330628974751</v>
+        <v>-3.55318096282316</v>
       </c>
       <c r="E172">
-        <v>-0.107231057421759</v>
+        <v>-0.1070813912701674</v>
       </c>
     </row>
     <row r="173" spans="1:5">
@@ -3327,10 +3327,10 @@
         <v>0.5</v>
       </c>
       <c r="D173">
-        <v>-3.58803688303712</v>
+        <v>-3.588130419252863</v>
       </c>
       <c r="E173">
-        <v>-0.1114577132835335</v>
+        <v>-0.111551249499277</v>
       </c>
     </row>
     <row r="174" spans="1:5">
@@ -3344,10 +3344,10 @@
         <v>0.6000000000000001</v>
       </c>
       <c r="D174">
-        <v>-3.615062663740765</v>
+        <v>-3.61408239373319</v>
       </c>
       <c r="E174">
-        <v>-0.1080038957865854</v>
+        <v>-0.1070236257790103</v>
       </c>
     </row>
     <row r="175" spans="1:5">
@@ -3361,10 +3361,10 @@
         <v>0.7000000000000001</v>
       </c>
       <c r="D175">
-        <v>-3.631835617047361</v>
+        <v>-3.632788154848153</v>
       </c>
       <c r="E175">
-        <v>-0.094297250892587</v>
+        <v>-0.09524978869337919</v>
       </c>
     </row>
     <row r="176" spans="1:5">
@@ -3378,10 +3378,10 @@
         <v>0.8</v>
       </c>
       <c r="D176">
-        <v>-3.641225162337584</v>
+        <v>-3.641543790124635</v>
       </c>
       <c r="E176">
-        <v>-0.07320719798221598</v>
+        <v>-0.07352582576926769</v>
       </c>
     </row>
     <row r="177" spans="1:5">
@@ -3395,10 +3395,10 @@
         <v>0.9</v>
       </c>
       <c r="D177">
-        <v>-3.642107052928966</v>
+        <v>-3.641427562512512</v>
       </c>
       <c r="E177">
-        <v>-0.04360949037300421</v>
+        <v>-0.04292999995655022</v>
       </c>
     </row>
     <row r="178" spans="1:5">
@@ -3446,10 +3446,10 @@
         <v>0.1</v>
       </c>
       <c r="D180">
-        <v>-3.408451116542633</v>
+        <v>-3.408965880232217</v>
       </c>
       <c r="E180">
-        <v>-0.04087492751618571</v>
+        <v>-0.04138969120576963</v>
       </c>
     </row>
     <row r="181" spans="1:5">
@@ -3463,10 +3463,10 @@
         <v>0.2</v>
       </c>
       <c r="D181">
-        <v>-3.469398272523909</v>
+        <v>-3.469972554759355</v>
       </c>
       <c r="E181">
-        <v>-0.07122513913378148</v>
+        <v>-0.07179942136922701</v>
       </c>
     </row>
     <row r="182" spans="1:5">
@@ -3480,10 +3480,10 @@
         <v>0.3</v>
       </c>
       <c r="D182">
-        <v>-3.522265696919604</v>
+        <v>-3.521615204898953</v>
       </c>
       <c r="E182">
-        <v>-0.09349561916579718</v>
+        <v>-0.09284512714514603</v>
       </c>
     </row>
     <row r="183" spans="1:5">
@@ -3497,10 +3497,10 @@
         <v>0.4</v>
       </c>
       <c r="D183">
-        <v>-3.566108172236689</v>
+        <v>-3.56535372207465</v>
       </c>
       <c r="E183">
-        <v>-0.1067411501192024</v>
+        <v>-0.1059866999571626</v>
       </c>
     </row>
     <row r="184" spans="1:5">
@@ -3514,10 +3514,10 @@
         <v>0.5</v>
       </c>
       <c r="D184">
-        <v>-3.599977080214474</v>
+        <v>-3.601358016121678</v>
       </c>
       <c r="E184">
-        <v>-0.1100131137333071</v>
+        <v>-0.1113940496405115</v>
       </c>
     </row>
     <row r="185" spans="1:5">
@@ -3531,10 +3531,10 @@
         <v>0.6000000000000001</v>
       </c>
       <c r="D185">
-        <v>-3.626486016514198</v>
+        <v>-3.626773133032127</v>
       </c>
       <c r="E185">
-        <v>-0.1059251056693506</v>
+        <v>-0.1062122221872794</v>
       </c>
     </row>
     <row r="186" spans="1:5">
@@ -3548,10 +3548,10 @@
         <v>0.7000000000000001</v>
       </c>
       <c r="D186">
-        <v>-3.64504240695338</v>
+        <v>-3.644419491887626</v>
       </c>
       <c r="E186">
-        <v>-0.09388455174485344</v>
+        <v>-0.09326163667909881</v>
       </c>
     </row>
     <row r="187" spans="1:5">
@@ -3565,10 +3565,10 @@
         <v>0.8</v>
       </c>
       <c r="D187">
-        <v>-3.653997728462638</v>
+        <v>-3.654226787667205</v>
       </c>
       <c r="E187">
-        <v>-0.07224292889043071</v>
+        <v>-0.07247198809499822</v>
       </c>
     </row>
     <row r="188" spans="1:5">
@@ -3582,10 +3582,10 @@
         <v>0.9</v>
       </c>
       <c r="D188">
-        <v>-3.655165113334387</v>
+        <v>-3.654240252498585</v>
       </c>
       <c r="E188">
-        <v>-0.04281336939850056</v>
+        <v>-0.04188850856269799</v>
       </c>
     </row>
     <row r="189" spans="1:5">
@@ -3602,6 +3602,380 @@
         <v>-3.642948688299567</v>
       </c>
       <c r="E189">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5">
+      <c r="A190">
+        <v>9841</v>
+      </c>
+      <c r="B190">
+        <v>4.693</v>
+      </c>
+      <c r="C190">
+        <v>0</v>
+      </c>
+      <c r="D190">
+        <v>-3.348562675651183</v>
+      </c>
+      <c r="E190">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5">
+      <c r="A191">
+        <v>9841</v>
+      </c>
+      <c r="B191">
+        <v>4.693</v>
+      </c>
+      <c r="C191">
+        <v>0.1</v>
+      </c>
+      <c r="D191">
+        <v>-3.420244583545085</v>
+      </c>
+      <c r="E191">
+        <v>-0.04097875442091281</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5">
+      <c r="A192">
+        <v>9841</v>
+      </c>
+      <c r="B192">
+        <v>4.693</v>
+      </c>
+      <c r="C192">
+        <v>0.2</v>
+      </c>
+      <c r="D192">
+        <v>-3.481371921097497</v>
+      </c>
+      <c r="E192">
+        <v>-0.07140293850033608</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5">
+      <c r="A193">
+        <v>9841</v>
+      </c>
+      <c r="B193">
+        <v>4.693</v>
+      </c>
+      <c r="C193">
+        <v>0.3</v>
+      </c>
+      <c r="D193">
+        <v>-3.533088530468241</v>
+      </c>
+      <c r="E193">
+        <v>-0.09241639439809157</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5">
+      <c r="A194">
+        <v>9841</v>
+      </c>
+      <c r="B194">
+        <v>4.693</v>
+      </c>
+      <c r="C194">
+        <v>0.4</v>
+      </c>
+      <c r="D194">
+        <v>-3.576826613235133</v>
+      </c>
+      <c r="E194">
+        <v>-0.1054513236919945</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5">
+      <c r="A195">
+        <v>9841</v>
+      </c>
+      <c r="B195">
+        <v>4.693</v>
+      </c>
+      <c r="C195">
+        <v>0.5</v>
+      </c>
+      <c r="D195">
+        <v>-3.612461579684119</v>
+      </c>
+      <c r="E195">
+        <v>-0.1103831366679922</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5">
+      <c r="A196">
+        <v>9841</v>
+      </c>
+      <c r="B196">
+        <v>4.693</v>
+      </c>
+      <c r="C196">
+        <v>0.6000000000000001</v>
+      </c>
+      <c r="D196">
+        <v>-3.638579885498066</v>
+      </c>
+      <c r="E196">
+        <v>-0.1057982890089508</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5">
+      <c r="A197">
+        <v>9841</v>
+      </c>
+      <c r="B197">
+        <v>4.693</v>
+      </c>
+      <c r="C197">
+        <v>0.7000000000000001</v>
+      </c>
+      <c r="D197">
+        <v>-3.65672800679553</v>
+      </c>
+      <c r="E197">
+        <v>-0.09324325683342516</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5">
+      <c r="A198">
+        <v>9841</v>
+      </c>
+      <c r="B198">
+        <v>4.693</v>
+      </c>
+      <c r="C198">
+        <v>0.8</v>
+      </c>
+      <c r="D198">
+        <v>-3.666303036992247</v>
+      </c>
+      <c r="E198">
+        <v>-0.07211513355715404</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5">
+      <c r="A199">
+        <v>9841</v>
+      </c>
+      <c r="B199">
+        <v>4.693</v>
+      </c>
+      <c r="C199">
+        <v>0.9</v>
+      </c>
+      <c r="D199">
+        <v>-3.66641810442219</v>
+      </c>
+      <c r="E199">
+        <v>-0.04152704751410813</v>
+      </c>
+    </row>
+    <row r="200" spans="1:5">
+      <c r="A200">
+        <v>9841</v>
+      </c>
+      <c r="B200">
+        <v>4.693</v>
+      </c>
+      <c r="C200">
+        <v>1</v>
+      </c>
+      <c r="D200">
+        <v>-3.655594210381071</v>
+      </c>
+      <c r="E200">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="201" spans="1:5">
+      <c r="A201">
+        <v>12195</v>
+      </c>
+      <c r="B201">
+        <v>5.054</v>
+      </c>
+      <c r="C201">
+        <v>0</v>
+      </c>
+      <c r="D201">
+        <v>-3.358019641371637</v>
+      </c>
+      <c r="E201">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5">
+      <c r="A202">
+        <v>12195</v>
+      </c>
+      <c r="B202">
+        <v>5.054</v>
+      </c>
+      <c r="C202">
+        <v>0.1</v>
+      </c>
+      <c r="D202">
+        <v>-3.429256390302887</v>
+      </c>
+      <c r="E202">
+        <v>-0.04044688402475005</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5">
+      <c r="A203">
+        <v>12195</v>
+      </c>
+      <c r="B203">
+        <v>5.054</v>
+      </c>
+      <c r="C203">
+        <v>0.2</v>
+      </c>
+      <c r="D203">
+        <v>-3.4900107672447</v>
+      </c>
+      <c r="E203">
+        <v>-0.07041139606006341</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5">
+      <c r="A204">
+        <v>12195</v>
+      </c>
+      <c r="B204">
+        <v>5.054</v>
+      </c>
+      <c r="C204">
+        <v>0.3</v>
+      </c>
+      <c r="D204">
+        <v>-3.542176825845236</v>
+      </c>
+      <c r="E204">
+        <v>-0.09178758975409851</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5">
+      <c r="A205">
+        <v>12195</v>
+      </c>
+      <c r="B205">
+        <v>5.054</v>
+      </c>
+      <c r="C205">
+        <v>0.4</v>
+      </c>
+      <c r="D205">
+        <v>-3.586248120689128</v>
+      </c>
+      <c r="E205">
+        <v>-0.1050690196914901</v>
+      </c>
+    </row>
+    <row r="206" spans="1:5">
+      <c r="A206">
+        <v>12195</v>
+      </c>
+      <c r="B206">
+        <v>5.054</v>
+      </c>
+      <c r="C206">
+        <v>0.5</v>
+      </c>
+      <c r="D206">
+        <v>-3.622074930838527</v>
+      </c>
+      <c r="E206">
+        <v>-0.1101059649343894</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5">
+      <c r="A207">
+        <v>12195</v>
+      </c>
+      <c r="B207">
+        <v>5.054</v>
+      </c>
+      <c r="C207">
+        <v>0.6000000000000001</v>
+      </c>
+      <c r="D207">
+        <v>-3.647313565695387</v>
+      </c>
+      <c r="E207">
+        <v>-0.1045547348847486</v>
+      </c>
+    </row>
+    <row r="208" spans="1:5">
+      <c r="A208">
+        <v>12195</v>
+      </c>
+      <c r="B208">
+        <v>5.054</v>
+      </c>
+      <c r="C208">
+        <v>0.7000000000000001</v>
+      </c>
+      <c r="D208">
+        <v>-3.665893747536095</v>
+      </c>
+      <c r="E208">
+        <v>-0.09234505181895658</v>
+      </c>
+    </row>
+    <row r="209" spans="1:5">
+      <c r="A209">
+        <v>12195</v>
+      </c>
+      <c r="B209">
+        <v>5.054</v>
+      </c>
+      <c r="C209">
+        <v>0.8</v>
+      </c>
+      <c r="D209">
+        <v>-3.675286250905322</v>
+      </c>
+      <c r="E209">
+        <v>-0.0709476902816838</v>
+      </c>
+    </row>
+    <row r="210" spans="1:5">
+      <c r="A210">
+        <v>12195</v>
+      </c>
+      <c r="B210">
+        <v>5.054</v>
+      </c>
+      <c r="C210">
+        <v>0.9</v>
+      </c>
+      <c r="D210">
+        <v>-3.676222316563647</v>
+      </c>
+      <c r="E210">
+        <v>-0.04109389103350819</v>
+      </c>
+    </row>
+    <row r="211" spans="1:5">
+      <c r="A211">
+        <v>12195</v>
+      </c>
+      <c r="B211">
+        <v>5.054</v>
+      </c>
+      <c r="C211">
+        <v>1</v>
+      </c>
+      <c r="D211">
+        <v>-3.665918290436639</v>
+      </c>
+      <c r="E211">
         <v>0</v>
       </c>
     </row>

</xml_diff>